<commit_message>
Changes made on 20/07/2023 at 20:24:01,66 from PC: DESKTOP-F6R5C8I
</commit_message>
<xml_diff>
--- a/courses.xlsx
+++ b/courses.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Notes\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A416D856-D168-4B03-BB34-7B7E2686E866}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C3006BBC-F2C3-4D4F-A3A6-5BB9313FE383}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -644,7 +644,7 @@
     <t>JavaScript Masterclass - Zero to Job-Ready with Hands-On Projects</t>
   </si>
   <si>
-    <t>JS</t>
+    <t>javascript</t>
   </si>
 </sst>
 </file>
@@ -686,7 +686,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -701,9 +701,6 @@
     <xf numFmtId="14" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
@@ -716,7 +713,8 @@
   </cellStyles>
   <dxfs count="15">
     <dxf>
-      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <numFmt numFmtId="0" formatCode="General"/>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
@@ -740,14 +738,13 @@
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
@@ -783,20 +780,20 @@
   <tableColumns count="14">
     <tableColumn id="4" xr3:uid="{4A213850-DE4B-4FE6-B4B5-91277FE7FF66}" name="year" dataDxfId="13"/>
     <tableColumn id="5" xr3:uid="{1DF95946-E7C7-4EEF-8374-81CBC97594F4}" name="plateform" dataDxfId="12"/>
-    <tableColumn id="16" xr3:uid="{7DD00BB8-229C-4796-93B5-A5F7BFC9AADD}" name="main subject" dataDxfId="2"/>
-    <tableColumn id="6" xr3:uid="{2A3E2F85-94E1-4138-8E16-ED7E54212EAF}" name="title" dataDxfId="0"/>
-    <tableColumn id="7" xr3:uid="{FB48243A-6764-4A7F-A85C-D0443CC1E609}" name="started at" dataDxfId="1"/>
-    <tableColumn id="8" xr3:uid="{09458720-1B8F-4611-B7DD-C25E4166F7D2}" name="finished at" dataDxfId="11"/>
-    <tableColumn id="15" xr3:uid="{A97B4FA4-E868-4D80-9513-BBC292926A04}" name="total sections" dataDxfId="10"/>
-    <tableColumn id="9" xr3:uid="{2E312EC2-08F1-4FEB-9E49-DA55B4987F10}" name="current section" dataDxfId="9"/>
-    <tableColumn id="10" xr3:uid="{4D640820-9D97-4ABF-A25F-66744C2A935E}" name="progress" dataDxfId="8">
+    <tableColumn id="16" xr3:uid="{7DD00BB8-229C-4796-93B5-A5F7BFC9AADD}" name="main subject" dataDxfId="11"/>
+    <tableColumn id="6" xr3:uid="{2A3E2F85-94E1-4138-8E16-ED7E54212EAF}" name="title" dataDxfId="10"/>
+    <tableColumn id="7" xr3:uid="{FB48243A-6764-4A7F-A85C-D0443CC1E609}" name="started at" dataDxfId="9"/>
+    <tableColumn id="8" xr3:uid="{09458720-1B8F-4611-B7DD-C25E4166F7D2}" name="finished at" dataDxfId="8"/>
+    <tableColumn id="15" xr3:uid="{A97B4FA4-E868-4D80-9513-BBC292926A04}" name="current section" dataDxfId="7"/>
+    <tableColumn id="9" xr3:uid="{2E312EC2-08F1-4FEB-9E49-DA55B4987F10}" name="total sections" dataDxfId="6"/>
+    <tableColumn id="10" xr3:uid="{4D640820-9D97-4ABF-A25F-66744C2A935E}" name="progress" dataDxfId="0">
       <calculatedColumnFormula>INT((Table1[[#This Row],[current section]]/Table1[[#This Row],[total sections]])*100)&amp;"%"</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="11" xr3:uid="{9CB6E5D8-27A7-487B-816B-136D644B5102}" name="notes" dataDxfId="7"/>
-    <tableColumn id="12" xr3:uid="{93D4FB50-FA3D-49E2-94CB-397269CE9100}" name="has_git" dataDxfId="6"/>
-    <tableColumn id="1" xr3:uid="{BD9254B6-01AD-4D11-A881-3FE1B369F6A7}" name="duration" dataDxfId="5"/>
-    <tableColumn id="2" xr3:uid="{56126BA6-8875-4EF0-8824-A3CBC2A59B71}" name="description" dataDxfId="4"/>
-    <tableColumn id="3" xr3:uid="{C243BCA3-96B3-417B-A11B-C44FF935B7D2}" name="author" dataDxfId="3"/>
+    <tableColumn id="11" xr3:uid="{9CB6E5D8-27A7-487B-816B-136D644B5102}" name="notes" dataDxfId="5"/>
+    <tableColumn id="12" xr3:uid="{93D4FB50-FA3D-49E2-94CB-397269CE9100}" name="has_git" dataDxfId="4"/>
+    <tableColumn id="1" xr3:uid="{BD9254B6-01AD-4D11-A881-3FE1B369F6A7}" name="duration" dataDxfId="3"/>
+    <tableColumn id="2" xr3:uid="{56126BA6-8875-4EF0-8824-A3CBC2A59B71}" name="description" dataDxfId="2"/>
+    <tableColumn id="3" xr3:uid="{C243BCA3-96B3-417B-A11B-C44FF935B7D2}" name="author" dataDxfId="1"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium16" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1111,8 +1108,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:N24"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
-      <selection activeCell="I26" sqref="I26"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="J29" sqref="J29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1150,10 +1147,10 @@
         <v>164</v>
       </c>
       <c r="G1" t="s">
+        <v>184</v>
+      </c>
+      <c r="H1" t="s">
         <v>183</v>
-      </c>
-      <c r="H1" t="s">
-        <v>184</v>
       </c>
       <c r="I1" t="s">
         <v>3</v>
@@ -1613,7 +1610,7 @@
       <c r="C15" s="4" t="s">
         <v>167</v>
       </c>
-      <c r="D15" s="7" t="s">
+      <c r="D15" s="6" t="s">
         <v>180</v>
       </c>
       <c r="E15" s="5" t="s">
@@ -1621,10 +1618,10 @@
       </c>
       <c r="F15" s="4"/>
       <c r="G15" s="4">
+        <v>8</v>
+      </c>
+      <c r="H15" s="4">
         <v>19</v>
-      </c>
-      <c r="H15" s="4">
-        <v>8</v>
       </c>
       <c r="I15" s="4" t="str">
         <f>INT((Table1[[#This Row],[current section]]/Table1[[#This Row],[total sections]])*100)&amp;"%"</f>
@@ -1915,19 +1912,19 @@
       <c r="D24" s="1" t="s">
         <v>202</v>
       </c>
-      <c r="E24" s="8">
+      <c r="E24" s="7">
         <v>45117</v>
       </c>
       <c r="F24" s="3"/>
       <c r="G24" s="3">
+        <v>3</v>
+      </c>
+      <c r="H24" s="3">
         <v>26</v>
       </c>
-      <c r="H24" s="3">
-        <v>2</v>
-      </c>
-      <c r="I24" s="6" t="str">
+      <c r="I24" s="3" t="str">
         <f>INT((Table1[[#This Row],[current section]]/Table1[[#This Row],[total sections]])*100)&amp;"%"</f>
-        <v>7%</v>
+        <v>11%</v>
       </c>
       <c r="J24" s="3"/>
       <c r="K24" s="3"/>

</xml_diff>

<commit_message>
Changes made on 20/07/2023 at 20:35:16,22 from PC Home
</commit_message>
<xml_diff>
--- a/courses.xlsx
+++ b/courses.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Notes\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C3006BBC-F2C3-4D4F-A3A6-5BB9313FE383}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{76631644-FFD5-42C7-A873-63AF4206682B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -713,7 +713,6 @@
   </cellStyles>
   <dxfs count="15">
     <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
@@ -729,6 +728,7 @@
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
@@ -786,14 +786,14 @@
     <tableColumn id="8" xr3:uid="{09458720-1B8F-4611-B7DD-C25E4166F7D2}" name="finished at" dataDxfId="8"/>
     <tableColumn id="15" xr3:uid="{A97B4FA4-E868-4D80-9513-BBC292926A04}" name="current section" dataDxfId="7"/>
     <tableColumn id="9" xr3:uid="{2E312EC2-08F1-4FEB-9E49-DA55B4987F10}" name="total sections" dataDxfId="6"/>
-    <tableColumn id="10" xr3:uid="{4D640820-9D97-4ABF-A25F-66744C2A935E}" name="progress" dataDxfId="0">
+    <tableColumn id="10" xr3:uid="{4D640820-9D97-4ABF-A25F-66744C2A935E}" name="progress" dataDxfId="5">
       <calculatedColumnFormula>INT((Table1[[#This Row],[current section]]/Table1[[#This Row],[total sections]])*100)&amp;"%"</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="11" xr3:uid="{9CB6E5D8-27A7-487B-816B-136D644B5102}" name="notes" dataDxfId="5"/>
-    <tableColumn id="12" xr3:uid="{93D4FB50-FA3D-49E2-94CB-397269CE9100}" name="has_git" dataDxfId="4"/>
-    <tableColumn id="1" xr3:uid="{BD9254B6-01AD-4D11-A881-3FE1B369F6A7}" name="duration" dataDxfId="3"/>
-    <tableColumn id="2" xr3:uid="{56126BA6-8875-4EF0-8824-A3CBC2A59B71}" name="description" dataDxfId="2"/>
-    <tableColumn id="3" xr3:uid="{C243BCA3-96B3-417B-A11B-C44FF935B7D2}" name="author" dataDxfId="1"/>
+    <tableColumn id="11" xr3:uid="{9CB6E5D8-27A7-487B-816B-136D644B5102}" name="notes" dataDxfId="4"/>
+    <tableColumn id="12" xr3:uid="{93D4FB50-FA3D-49E2-94CB-397269CE9100}" name="has_git" dataDxfId="3"/>
+    <tableColumn id="1" xr3:uid="{BD9254B6-01AD-4D11-A881-3FE1B369F6A7}" name="duration" dataDxfId="2"/>
+    <tableColumn id="2" xr3:uid="{56126BA6-8875-4EF0-8824-A3CBC2A59B71}" name="description" dataDxfId="1"/>
+    <tableColumn id="3" xr3:uid="{C243BCA3-96B3-417B-A11B-C44FF935B7D2}" name="author" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium16" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1109,7 +1109,7 @@
   <dimension ref="A1:N24"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J29" sqref="J29"/>
+      <selection activeCell="L24" sqref="L24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1928,7 +1928,10 @@
       </c>
       <c r="J24" s="3"/>
       <c r="K24" s="3"/>
-      <c r="L24" s="3"/>
+      <c r="L24" s="3">
+        <f>-L31</f>
+        <v>0</v>
+      </c>
       <c r="M24" s="3"/>
       <c r="N24" s="3" t="s">
         <v>146</v>

</xml_diff>

<commit_message>
Changes made on 22/07/2023 at 15:43:14,32 from PC Home
</commit_message>
<xml_diff>
--- a/courses.xlsx
+++ b/courses.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Notes\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{76631644-FFD5-42C7-A873-63AF4206682B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{30B453AE-D6CC-4FCE-80E0-FFB144A4D2E2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="327" uniqueCount="204">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="329" uniqueCount="204">
   <si>
     <t>duration</t>
   </si>
@@ -686,7 +686,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -704,14 +704,14 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="15">
+  <dxfs count="16">
+    <dxf>
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
     <dxf>
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
@@ -772,28 +772,29 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{F5801A2D-4A6C-4794-B5C6-BD54C875A28D}" name="Table1" displayName="Table1" ref="A1:N24" totalsRowShown="0" dataDxfId="14">
-  <autoFilter ref="A1:N24" xr:uid="{F5801A2D-4A6C-4794-B5C6-BD54C875A28D}"/>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:N23">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{F5801A2D-4A6C-4794-B5C6-BD54C875A28D}" name="Table1" displayName="Table1" ref="A1:O24" totalsRowShown="0" dataDxfId="15">
+  <autoFilter ref="A1:O24" xr:uid="{F5801A2D-4A6C-4794-B5C6-BD54C875A28D}"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:O23">
     <sortCondition ref="C1:C23"/>
   </sortState>
-  <tableColumns count="14">
-    <tableColumn id="4" xr3:uid="{4A213850-DE4B-4FE6-B4B5-91277FE7FF66}" name="year" dataDxfId="13"/>
-    <tableColumn id="5" xr3:uid="{1DF95946-E7C7-4EEF-8374-81CBC97594F4}" name="plateform" dataDxfId="12"/>
-    <tableColumn id="16" xr3:uid="{7DD00BB8-229C-4796-93B5-A5F7BFC9AADD}" name="main subject" dataDxfId="11"/>
-    <tableColumn id="6" xr3:uid="{2A3E2F85-94E1-4138-8E16-ED7E54212EAF}" name="title" dataDxfId="10"/>
-    <tableColumn id="7" xr3:uid="{FB48243A-6764-4A7F-A85C-D0443CC1E609}" name="started at" dataDxfId="9"/>
-    <tableColumn id="8" xr3:uid="{09458720-1B8F-4611-B7DD-C25E4166F7D2}" name="finished at" dataDxfId="8"/>
-    <tableColumn id="15" xr3:uid="{A97B4FA4-E868-4D80-9513-BBC292926A04}" name="current section" dataDxfId="7"/>
-    <tableColumn id="9" xr3:uid="{2E312EC2-08F1-4FEB-9E49-DA55B4987F10}" name="total sections" dataDxfId="6"/>
-    <tableColumn id="10" xr3:uid="{4D640820-9D97-4ABF-A25F-66744C2A935E}" name="progress" dataDxfId="5">
+  <tableColumns count="15">
+    <tableColumn id="4" xr3:uid="{4A213850-DE4B-4FE6-B4B5-91277FE7FF66}" name="year" dataDxfId="14"/>
+    <tableColumn id="5" xr3:uid="{1DF95946-E7C7-4EEF-8374-81CBC97594F4}" name="plateform" dataDxfId="13"/>
+    <tableColumn id="16" xr3:uid="{7DD00BB8-229C-4796-93B5-A5F7BFC9AADD}" name="main subject" dataDxfId="12"/>
+    <tableColumn id="6" xr3:uid="{2A3E2F85-94E1-4138-8E16-ED7E54212EAF}" name="title" dataDxfId="11"/>
+    <tableColumn id="13" xr3:uid="{48F1BD13-876C-498D-A84D-9C92899C1E8A}" name="current lecture" dataDxfId="0"/>
+    <tableColumn id="7" xr3:uid="{FB48243A-6764-4A7F-A85C-D0443CC1E609}" name="started at" dataDxfId="10"/>
+    <tableColumn id="8" xr3:uid="{09458720-1B8F-4611-B7DD-C25E4166F7D2}" name="finished at" dataDxfId="9"/>
+    <tableColumn id="15" xr3:uid="{A97B4FA4-E868-4D80-9513-BBC292926A04}" name="current section" dataDxfId="8"/>
+    <tableColumn id="9" xr3:uid="{2E312EC2-08F1-4FEB-9E49-DA55B4987F10}" name="total sections" dataDxfId="7"/>
+    <tableColumn id="10" xr3:uid="{4D640820-9D97-4ABF-A25F-66744C2A935E}" name="progress" dataDxfId="6">
       <calculatedColumnFormula>INT((Table1[[#This Row],[current section]]/Table1[[#This Row],[total sections]])*100)&amp;"%"</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="11" xr3:uid="{9CB6E5D8-27A7-487B-816B-136D644B5102}" name="notes" dataDxfId="4"/>
-    <tableColumn id="12" xr3:uid="{93D4FB50-FA3D-49E2-94CB-397269CE9100}" name="has_git" dataDxfId="3"/>
-    <tableColumn id="1" xr3:uid="{BD9254B6-01AD-4D11-A881-3FE1B369F6A7}" name="duration" dataDxfId="2"/>
-    <tableColumn id="2" xr3:uid="{56126BA6-8875-4EF0-8824-A3CBC2A59B71}" name="description" dataDxfId="1"/>
-    <tableColumn id="3" xr3:uid="{C243BCA3-96B3-417B-A11B-C44FF935B7D2}" name="author" dataDxfId="0"/>
+    <tableColumn id="11" xr3:uid="{9CB6E5D8-27A7-487B-816B-136D644B5102}" name="notes" dataDxfId="5"/>
+    <tableColumn id="12" xr3:uid="{93D4FB50-FA3D-49E2-94CB-397269CE9100}" name="has_git" dataDxfId="4"/>
+    <tableColumn id="1" xr3:uid="{BD9254B6-01AD-4D11-A881-3FE1B369F6A7}" name="duration" dataDxfId="3"/>
+    <tableColumn id="2" xr3:uid="{56126BA6-8875-4EF0-8824-A3CBC2A59B71}" name="description" dataDxfId="2"/>
+    <tableColumn id="3" xr3:uid="{C243BCA3-96B3-417B-A11B-C44FF935B7D2}" name="author" dataDxfId="1"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium16" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1106,10 +1107,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:N24"/>
+  <dimension ref="A1:O24"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L24" sqref="L24"/>
+      <selection activeCell="G32" sqref="G32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1118,16 +1119,18 @@
     <col min="2" max="2" width="10.85546875" customWidth="1"/>
     <col min="3" max="3" width="14" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="60.7109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="12.85546875" customWidth="1"/>
-    <col min="6" max="7" width="11.28515625" customWidth="1"/>
-    <col min="8" max="8" width="14.85546875" customWidth="1"/>
-    <col min="9" max="9" width="9.7109375" customWidth="1"/>
-    <col min="12" max="12" width="13.42578125" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="105.28515625" customWidth="1"/>
-    <col min="14" max="14" width="34.7109375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="30.42578125" style="1" customWidth="1"/>
+    <col min="6" max="6" width="12.85546875" customWidth="1"/>
+    <col min="7" max="7" width="11.28515625" customWidth="1"/>
+    <col min="8" max="8" width="6.5703125" customWidth="1"/>
+    <col min="9" max="9" width="6.85546875" customWidth="1"/>
+    <col min="10" max="10" width="9.7109375" customWidth="1"/>
+    <col min="13" max="13" width="13.42578125" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="105.28515625" customWidth="1"/>
+    <col min="15" max="15" width="34.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>160</v>
       </c>
@@ -1140,38 +1143,41 @@
       <c r="D1" s="1" t="s">
         <v>162</v>
       </c>
-      <c r="E1" t="s">
+      <c r="E1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="F1" t="s">
         <v>163</v>
       </c>
-      <c r="F1" t="s">
+      <c r="G1" t="s">
         <v>164</v>
       </c>
-      <c r="G1" t="s">
+      <c r="H1" t="s">
         <v>184</v>
       </c>
-      <c r="H1" t="s">
+      <c r="I1" t="s">
         <v>183</v>
       </c>
-      <c r="I1" t="s">
+      <c r="J1" t="s">
         <v>3</v>
       </c>
-      <c r="J1" t="s">
+      <c r="K1" t="s">
         <v>4</v>
       </c>
-      <c r="K1" t="s">
+      <c r="L1" t="s">
         <v>5</v>
       </c>
-      <c r="L1" t="s">
+      <c r="M1" t="s">
         <v>0</v>
       </c>
-      <c r="M1" t="s">
+      <c r="N1" t="s">
         <v>6</v>
       </c>
-      <c r="N1" t="s">
+      <c r="O1" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
         <v>79</v>
       </c>
@@ -1184,27 +1190,27 @@
       <c r="D2" s="1" t="s">
         <v>150</v>
       </c>
-      <c r="E2" s="3"/>
       <c r="F2" s="3"/>
       <c r="G2" s="3"/>
       <c r="H2" s="3"/>
-      <c r="I2" s="3" t="e">
+      <c r="I2" s="3"/>
+      <c r="J2" s="3" t="e">
         <f>INT((Table1[[#This Row],[current section]]/Table1[[#This Row],[total sections]])*100)&amp;"%"</f>
         <v>#DIV/0!</v>
       </c>
-      <c r="J2" s="3"/>
       <c r="K2" s="3"/>
-      <c r="L2" s="3" t="s">
+      <c r="L2" s="3"/>
+      <c r="M2" s="3" t="s">
         <v>148</v>
       </c>
-      <c r="M2" s="3" t="s">
+      <c r="N2" s="3" t="s">
         <v>149</v>
       </c>
-      <c r="N2" s="3" t="s">
+      <c r="O2" s="3" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="3" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="s">
         <v>20</v>
       </c>
@@ -1217,27 +1223,27 @@
       <c r="D3" s="1" t="s">
         <v>137</v>
       </c>
-      <c r="E3" s="3"/>
       <c r="F3" s="3"/>
       <c r="G3" s="3"/>
       <c r="H3" s="3"/>
-      <c r="I3" s="3" t="e">
+      <c r="I3" s="3"/>
+      <c r="J3" s="3" t="e">
         <f>INT((Table1[[#This Row],[current section]]/Table1[[#This Row],[total sections]])*100)&amp;"%"</f>
         <v>#DIV/0!</v>
       </c>
-      <c r="J3" s="3"/>
       <c r="K3" s="3"/>
-      <c r="L3" s="3" t="s">
+      <c r="L3" s="3"/>
+      <c r="M3" s="3" t="s">
         <v>134</v>
       </c>
-      <c r="M3" s="3" t="s">
+      <c r="N3" s="3" t="s">
         <v>135</v>
       </c>
-      <c r="N3" s="3" t="s">
+      <c r="O3" s="3" t="s">
         <v>136</v>
       </c>
     </row>
-    <row r="4" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A4" s="3" t="s">
         <v>30</v>
       </c>
@@ -1250,27 +1256,27 @@
       <c r="D4" s="1" t="s">
         <v>185</v>
       </c>
-      <c r="E4" s="3"/>
       <c r="F4" s="3"/>
       <c r="G4" s="3"/>
       <c r="H4" s="3"/>
-      <c r="I4" s="3" t="e">
+      <c r="I4" s="3"/>
+      <c r="J4" s="3" t="e">
         <f>INT((Table1[[#This Row],[current section]]/Table1[[#This Row],[total sections]])*100)&amp;"%"</f>
         <v>#DIV/0!</v>
       </c>
-      <c r="J4" s="3"/>
       <c r="K4" s="3"/>
-      <c r="L4" s="3" t="s">
+      <c r="L4" s="3"/>
+      <c r="M4" s="3" t="s">
         <v>97</v>
       </c>
-      <c r="M4" s="3" t="s">
+      <c r="N4" s="3" t="s">
         <v>98</v>
       </c>
-      <c r="N4" s="3" t="s">
+      <c r="O4" s="3" t="s">
         <v>99</v>
       </c>
     </row>
-    <row r="5" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A5" s="3" t="s">
         <v>35</v>
       </c>
@@ -1283,27 +1289,27 @@
       <c r="D5" s="1" t="s">
         <v>197</v>
       </c>
-      <c r="E5" s="3"/>
       <c r="F5" s="3"/>
       <c r="G5" s="3"/>
       <c r="H5" s="3"/>
-      <c r="I5" s="3" t="e">
+      <c r="I5" s="3"/>
+      <c r="J5" s="3" t="e">
         <f>INT((Table1[[#This Row],[current section]]/Table1[[#This Row],[total sections]])*100)&amp;"%"</f>
         <v>#DIV/0!</v>
       </c>
-      <c r="J5" s="3"/>
       <c r="K5" s="3"/>
-      <c r="L5" s="3" t="s">
+      <c r="L5" s="3"/>
+      <c r="M5" s="3" t="s">
         <v>103</v>
       </c>
-      <c r="M5" s="3" t="s">
+      <c r="N5" s="3" t="s">
         <v>104</v>
       </c>
-      <c r="N5" s="3" t="s">
+      <c r="O5" s="3" t="s">
         <v>105</v>
       </c>
     </row>
-    <row r="6" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A6" s="3" t="s">
         <v>25</v>
       </c>
@@ -1316,27 +1322,27 @@
       <c r="D6" s="1" t="s">
         <v>196</v>
       </c>
-      <c r="E6" s="3"/>
       <c r="F6" s="3"/>
       <c r="G6" s="3"/>
       <c r="H6" s="3"/>
-      <c r="I6" s="3" t="e">
+      <c r="I6" s="3"/>
+      <c r="J6" s="3" t="e">
         <f>INT((Table1[[#This Row],[current section]]/Table1[[#This Row],[total sections]])*100)&amp;"%"</f>
         <v>#DIV/0!</v>
       </c>
-      <c r="J6" s="3"/>
       <c r="K6" s="3"/>
-      <c r="L6" s="3" t="s">
+      <c r="L6" s="3"/>
+      <c r="M6" s="3" t="s">
         <v>131</v>
       </c>
-      <c r="M6" s="3" t="s">
+      <c r="N6" s="3" t="s">
         <v>132</v>
       </c>
-      <c r="N6" s="3" t="s">
+      <c r="O6" s="3" t="s">
         <v>133</v>
       </c>
     </row>
-    <row r="7" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A7" s="3" t="s">
         <v>10</v>
       </c>
@@ -1349,27 +1355,27 @@
       <c r="D7" s="1" t="s">
         <v>186</v>
       </c>
-      <c r="E7" s="3"/>
       <c r="F7" s="3"/>
       <c r="G7" s="3"/>
       <c r="H7" s="3"/>
-      <c r="I7" s="3" t="e">
+      <c r="I7" s="3"/>
+      <c r="J7" s="3" t="e">
         <f>INT((Table1[[#This Row],[current section]]/Table1[[#This Row],[total sections]])*100)&amp;"%"</f>
         <v>#DIV/0!</v>
       </c>
-      <c r="J7" s="3"/>
       <c r="K7" s="3"/>
-      <c r="L7" s="3" t="s">
+      <c r="L7" s="3"/>
+      <c r="M7" s="3" t="s">
         <v>157</v>
       </c>
-      <c r="M7" s="3" t="s">
+      <c r="N7" s="3" t="s">
         <v>158</v>
       </c>
-      <c r="N7" s="3" t="s">
+      <c r="O7" s="3" t="s">
         <v>159</v>
       </c>
     </row>
-    <row r="8" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A8" s="3" t="s">
         <v>35</v>
       </c>
@@ -1382,27 +1388,27 @@
       <c r="D8" s="1" t="s">
         <v>125</v>
       </c>
-      <c r="E8" s="3"/>
       <c r="F8" s="3"/>
       <c r="G8" s="3"/>
       <c r="H8" s="3"/>
-      <c r="I8" s="3" t="e">
+      <c r="I8" s="3"/>
+      <c r="J8" s="3" t="e">
         <f>INT((Table1[[#This Row],[current section]]/Table1[[#This Row],[total sections]])*100)&amp;"%"</f>
         <v>#DIV/0!</v>
       </c>
-      <c r="J8" s="3"/>
       <c r="K8" s="3"/>
-      <c r="L8" s="3" t="s">
+      <c r="L8" s="3"/>
+      <c r="M8" s="3" t="s">
         <v>122</v>
       </c>
-      <c r="M8" s="3" t="s">
+      <c r="N8" s="3" t="s">
         <v>123</v>
       </c>
-      <c r="N8" s="3" t="s">
+      <c r="O8" s="3" t="s">
         <v>124</v>
       </c>
     </row>
-    <row r="9" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A9" s="3" t="s">
         <v>35</v>
       </c>
@@ -1415,27 +1421,27 @@
       <c r="D9" s="1" t="s">
         <v>187</v>
       </c>
-      <c r="E9" s="3"/>
       <c r="F9" s="3"/>
       <c r="G9" s="3"/>
       <c r="H9" s="3"/>
-      <c r="I9" s="3" t="e">
+      <c r="I9" s="3"/>
+      <c r="J9" s="3" t="e">
         <f>INT((Table1[[#This Row],[current section]]/Table1[[#This Row],[total sections]])*100)&amp;"%"</f>
         <v>#DIV/0!</v>
       </c>
-      <c r="J9" s="3"/>
       <c r="K9" s="3"/>
-      <c r="L9" s="3" t="s">
+      <c r="L9" s="3"/>
+      <c r="M9" s="3" t="s">
         <v>142</v>
       </c>
-      <c r="M9" s="3" t="s">
+      <c r="N9" s="3" t="s">
         <v>143</v>
       </c>
-      <c r="N9" s="3" t="s">
+      <c r="O9" s="3" t="s">
         <v>105</v>
       </c>
     </row>
-    <row r="10" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A10" s="3" t="s">
         <v>25</v>
       </c>
@@ -1448,27 +1454,27 @@
       <c r="D10" s="1" t="s">
         <v>188</v>
       </c>
-      <c r="E10" s="3"/>
       <c r="F10" s="3"/>
       <c r="G10" s="3"/>
       <c r="H10" s="3"/>
-      <c r="I10" s="3" t="e">
+      <c r="I10" s="3"/>
+      <c r="J10" s="3" t="e">
         <f>INT((Table1[[#This Row],[current section]]/Table1[[#This Row],[total sections]])*100)&amp;"%"</f>
         <v>#DIV/0!</v>
       </c>
-      <c r="J10" s="3"/>
       <c r="K10" s="3"/>
-      <c r="L10" s="3" t="s">
+      <c r="L10" s="3"/>
+      <c r="M10" s="3" t="s">
         <v>140</v>
       </c>
-      <c r="M10" s="3" t="s">
+      <c r="N10" s="3" t="s">
         <v>141</v>
       </c>
-      <c r="N10" s="3" t="s">
+      <c r="O10" s="3" t="s">
         <v>124</v>
       </c>
     </row>
-    <row r="11" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A11" s="3" t="s">
         <v>25</v>
       </c>
@@ -1481,27 +1487,27 @@
       <c r="D11" s="1" t="s">
         <v>189</v>
       </c>
-      <c r="E11" s="3"/>
       <c r="F11" s="3"/>
       <c r="G11" s="3"/>
       <c r="H11" s="3"/>
-      <c r="I11" s="3" t="e">
+      <c r="I11" s="3"/>
+      <c r="J11" s="3" t="e">
         <f>INT((Table1[[#This Row],[current section]]/Table1[[#This Row],[total sections]])*100)&amp;"%"</f>
         <v>#DIV/0!</v>
       </c>
-      <c r="J11" s="3"/>
       <c r="K11" s="3"/>
-      <c r="L11" s="3" t="s">
+      <c r="L11" s="3"/>
+      <c r="M11" s="3" t="s">
         <v>138</v>
       </c>
-      <c r="M11" s="3" t="s">
+      <c r="N11" s="3" t="s">
         <v>139</v>
       </c>
-      <c r="N11" s="3" t="s">
+      <c r="O11" s="3" t="s">
         <v>124</v>
       </c>
     </row>
-    <row r="12" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A12" s="3" t="s">
         <v>25</v>
       </c>
@@ -1514,27 +1520,27 @@
       <c r="D12" s="1" t="s">
         <v>114</v>
       </c>
-      <c r="E12" s="3"/>
       <c r="F12" s="3"/>
       <c r="G12" s="3"/>
       <c r="H12" s="3"/>
-      <c r="I12" s="3" t="e">
+      <c r="I12" s="3"/>
+      <c r="J12" s="3" t="e">
         <f>INT((Table1[[#This Row],[current section]]/Table1[[#This Row],[total sections]])*100)&amp;"%"</f>
         <v>#DIV/0!</v>
       </c>
-      <c r="J12" s="3"/>
       <c r="K12" s="3"/>
-      <c r="L12" s="3" t="s">
+      <c r="L12" s="3"/>
+      <c r="M12" s="3" t="s">
         <v>111</v>
       </c>
-      <c r="M12" s="3" t="s">
+      <c r="N12" s="3" t="s">
         <v>112</v>
       </c>
-      <c r="N12" s="3" t="s">
+      <c r="O12" s="3" t="s">
         <v>113</v>
       </c>
     </row>
-    <row r="13" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A13" s="3" t="s">
         <v>79</v>
       </c>
@@ -1547,27 +1553,27 @@
       <c r="D13" s="1" t="s">
         <v>190</v>
       </c>
-      <c r="E13" s="3"/>
       <c r="F13" s="3"/>
       <c r="G13" s="3"/>
       <c r="H13" s="3"/>
-      <c r="I13" s="3" t="e">
+      <c r="I13" s="3"/>
+      <c r="J13" s="3" t="e">
         <f>INT((Table1[[#This Row],[current section]]/Table1[[#This Row],[total sections]])*100)&amp;"%"</f>
         <v>#DIV/0!</v>
       </c>
-      <c r="J13" s="3"/>
       <c r="K13" s="3"/>
-      <c r="L13" s="3" t="s">
+      <c r="L13" s="3"/>
+      <c r="M13" s="3" t="s">
         <v>126</v>
       </c>
-      <c r="M13" s="3" t="s">
+      <c r="N13" s="3" t="s">
         <v>127</v>
       </c>
-      <c r="N13" s="3" t="s">
+      <c r="O13" s="3" t="s">
         <v>117</v>
       </c>
     </row>
-    <row r="14" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A14" s="3" t="s">
         <v>25</v>
       </c>
@@ -1580,27 +1586,27 @@
       <c r="D14" s="1" t="s">
         <v>156</v>
       </c>
-      <c r="E14" s="3"/>
       <c r="F14" s="3"/>
       <c r="G14" s="3"/>
       <c r="H14" s="3"/>
-      <c r="I14" s="3" t="e">
+      <c r="I14" s="3"/>
+      <c r="J14" s="3" t="e">
         <f>INT((Table1[[#This Row],[current section]]/Table1[[#This Row],[total sections]])*100)&amp;"%"</f>
         <v>#DIV/0!</v>
       </c>
-      <c r="J14" s="3"/>
       <c r="K14" s="3"/>
-      <c r="L14" s="3" t="s">
+      <c r="L14" s="3"/>
+      <c r="M14" s="3" t="s">
         <v>154</v>
       </c>
-      <c r="M14" s="3" t="s">
+      <c r="N14" s="3" t="s">
         <v>155</v>
       </c>
-      <c r="N14" s="3" t="s">
+      <c r="O14" s="3" t="s">
         <v>136</v>
       </c>
     </row>
-    <row r="15" spans="1:14" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:15" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A15" s="4">
         <v>2023</v>
       </c>
@@ -1613,37 +1619,38 @@
       <c r="D15" s="6" t="s">
         <v>180</v>
       </c>
-      <c r="E15" s="5" t="s">
+      <c r="E15" s="6"/>
+      <c r="F15" s="5" t="s">
         <v>181</v>
       </c>
-      <c r="F15" s="4"/>
-      <c r="G15" s="4">
+      <c r="G15" s="4"/>
+      <c r="H15" s="4">
         <v>8</v>
       </c>
-      <c r="H15" s="4">
+      <c r="I15" s="4">
         <v>19</v>
       </c>
-      <c r="I15" s="4" t="str">
+      <c r="J15" s="4" t="str">
         <f>INT((Table1[[#This Row],[current section]]/Table1[[#This Row],[total sections]])*100)&amp;"%"</f>
         <v>42%</v>
       </c>
-      <c r="J15" s="4">
+      <c r="K15" s="4">
         <v>10</v>
       </c>
-      <c r="K15" s="4" t="s">
+      <c r="L15" s="4" t="s">
         <v>182</v>
       </c>
-      <c r="L15" s="4" t="s">
+      <c r="M15" s="4" t="s">
         <v>178</v>
       </c>
-      <c r="M15" s="4" t="s">
+      <c r="N15" s="4" t="s">
         <v>179</v>
       </c>
-      <c r="N15" s="4" t="s">
+      <c r="O15" s="4" t="s">
         <v>146</v>
       </c>
     </row>
-    <row r="16" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A16" s="3" t="s">
         <v>25</v>
       </c>
@@ -1656,27 +1663,27 @@
       <c r="D16" s="1" t="s">
         <v>191</v>
       </c>
-      <c r="E16" s="3"/>
       <c r="F16" s="3"/>
       <c r="G16" s="3"/>
       <c r="H16" s="3"/>
-      <c r="I16" s="3" t="e">
+      <c r="I16" s="3"/>
+      <c r="J16" s="3" t="e">
         <f>INT((Table1[[#This Row],[current section]]/Table1[[#This Row],[total sections]])*100)&amp;"%"</f>
         <v>#DIV/0!</v>
       </c>
-      <c r="J16" s="3"/>
       <c r="K16" s="3"/>
-      <c r="L16" s="3" t="s">
+      <c r="L16" s="3"/>
+      <c r="M16" s="3" t="s">
         <v>106</v>
       </c>
-      <c r="M16" s="3" t="s">
+      <c r="N16" s="3" t="s">
         <v>107</v>
       </c>
-      <c r="N16" s="3" t="s">
+      <c r="O16" s="3" t="s">
         <v>108</v>
       </c>
     </row>
-    <row r="17" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A17" s="3">
         <v>2020</v>
       </c>
@@ -1689,27 +1696,27 @@
       <c r="D17" s="1" t="s">
         <v>192</v>
       </c>
-      <c r="E17" s="3"/>
       <c r="F17" s="3"/>
       <c r="G17" s="3"/>
       <c r="H17" s="3"/>
-      <c r="I17" s="3" t="e">
+      <c r="I17" s="3"/>
+      <c r="J17" s="3" t="e">
         <f>INT((Table1[[#This Row],[current section]]/Table1[[#This Row],[total sections]])*100)&amp;"%"</f>
         <v>#DIV/0!</v>
       </c>
-      <c r="J17" s="3"/>
       <c r="K17" s="3"/>
-      <c r="L17" s="3" t="s">
+      <c r="L17" s="3"/>
+      <c r="M17" s="3" t="s">
         <v>109</v>
       </c>
-      <c r="M17" s="3" t="s">
+      <c r="N17" s="3" t="s">
         <v>110</v>
       </c>
-      <c r="N17" s="3" t="s">
+      <c r="O17" s="3" t="s">
         <v>108</v>
       </c>
     </row>
-    <row r="18" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A18" s="3" t="s">
         <v>79</v>
       </c>
@@ -1722,27 +1729,27 @@
       <c r="D18" s="1" t="s">
         <v>193</v>
       </c>
-      <c r="E18" s="3"/>
       <c r="F18" s="3"/>
       <c r="G18" s="3"/>
       <c r="H18" s="3"/>
-      <c r="I18" s="3" t="e">
+      <c r="I18" s="3"/>
+      <c r="J18" s="3" t="e">
         <f>INT((Table1[[#This Row],[current section]]/Table1[[#This Row],[total sections]])*100)&amp;"%"</f>
         <v>#DIV/0!</v>
       </c>
-      <c r="J18" s="3"/>
       <c r="K18" s="3"/>
-      <c r="L18" s="3" t="s">
+      <c r="L18" s="3"/>
+      <c r="M18" s="3" t="s">
         <v>128</v>
       </c>
-      <c r="M18" s="3" t="s">
+      <c r="N18" s="3" t="s">
         <v>129</v>
       </c>
-      <c r="N18" s="3" t="s">
+      <c r="O18" s="3" t="s">
         <v>130</v>
       </c>
     </row>
-    <row r="19" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A19" s="3" t="s">
         <v>35</v>
       </c>
@@ -1755,27 +1762,27 @@
       <c r="D19" s="1" t="s">
         <v>194</v>
       </c>
-      <c r="E19" s="3"/>
       <c r="F19" s="3"/>
       <c r="G19" s="3"/>
       <c r="H19" s="3"/>
-      <c r="I19" s="3" t="e">
+      <c r="I19" s="3"/>
+      <c r="J19" s="3" t="e">
         <f>INT((Table1[[#This Row],[current section]]/Table1[[#This Row],[total sections]])*100)&amp;"%"</f>
         <v>#DIV/0!</v>
       </c>
-      <c r="J19" s="3"/>
       <c r="K19" s="3"/>
-      <c r="L19" s="3" t="s">
+      <c r="L19" s="3"/>
+      <c r="M19" s="3" t="s">
         <v>100</v>
       </c>
-      <c r="M19" s="3" t="s">
+      <c r="N19" s="3" t="s">
         <v>101</v>
       </c>
-      <c r="N19" s="3" t="s">
+      <c r="O19" s="3" t="s">
         <v>102</v>
       </c>
     </row>
-    <row r="20" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A20" s="3" t="s">
         <v>79</v>
       </c>
@@ -1786,27 +1793,27 @@
       <c r="D20" s="1" t="s">
         <v>118</v>
       </c>
-      <c r="E20" s="3"/>
       <c r="F20" s="3"/>
       <c r="G20" s="3"/>
       <c r="H20" s="3"/>
-      <c r="I20" s="3" t="e">
+      <c r="I20" s="3"/>
+      <c r="J20" s="3" t="e">
         <f>INT((Table1[[#This Row],[current section]]/Table1[[#This Row],[total sections]])*100)&amp;"%"</f>
         <v>#DIV/0!</v>
       </c>
-      <c r="J20" s="3"/>
       <c r="K20" s="3"/>
-      <c r="L20" s="3" t="s">
+      <c r="L20" s="3"/>
+      <c r="M20" s="3" t="s">
         <v>115</v>
       </c>
-      <c r="M20" s="3" t="s">
+      <c r="N20" s="3" t="s">
         <v>116</v>
       </c>
-      <c r="N20" s="3" t="s">
+      <c r="O20" s="3" t="s">
         <v>117</v>
       </c>
     </row>
-    <row r="21" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A21" s="3" t="s">
         <v>25</v>
       </c>
@@ -1817,27 +1824,27 @@
       <c r="D21" s="1" t="s">
         <v>147</v>
       </c>
-      <c r="E21" s="3"/>
       <c r="F21" s="3"/>
       <c r="G21" s="3"/>
       <c r="H21" s="3"/>
-      <c r="I21" s="3" t="e">
+      <c r="I21" s="3"/>
+      <c r="J21" s="3" t="e">
         <f>INT((Table1[[#This Row],[current section]]/Table1[[#This Row],[total sections]])*100)&amp;"%"</f>
         <v>#DIV/0!</v>
       </c>
-      <c r="J21" s="3"/>
       <c r="K21" s="3"/>
-      <c r="L21" s="3" t="s">
+      <c r="L21" s="3"/>
+      <c r="M21" s="3" t="s">
         <v>144</v>
       </c>
-      <c r="M21" s="3" t="s">
+      <c r="N21" s="3" t="s">
         <v>145</v>
       </c>
-      <c r="N21" s="3" t="s">
+      <c r="O21" s="3" t="s">
         <v>146</v>
       </c>
     </row>
-    <row r="22" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A22" s="3" t="s">
         <v>25</v>
       </c>
@@ -1848,27 +1855,27 @@
       <c r="D22" s="1" t="s">
         <v>153</v>
       </c>
-      <c r="E22" s="3"/>
       <c r="F22" s="3"/>
       <c r="G22" s="3"/>
       <c r="H22" s="3"/>
-      <c r="I22" s="3" t="e">
+      <c r="I22" s="3"/>
+      <c r="J22" s="3" t="e">
         <f>INT((Table1[[#This Row],[current section]]/Table1[[#This Row],[total sections]])*100)&amp;"%"</f>
         <v>#DIV/0!</v>
       </c>
-      <c r="J22" s="3"/>
       <c r="K22" s="3"/>
-      <c r="L22" s="3" t="s">
+      <c r="L22" s="3"/>
+      <c r="M22" s="3" t="s">
         <v>151</v>
       </c>
-      <c r="M22" s="3" t="s">
+      <c r="N22" s="3" t="s">
         <v>152</v>
       </c>
-      <c r="N22" s="3" t="s">
+      <c r="O22" s="3" t="s">
         <v>113</v>
       </c>
     </row>
-    <row r="23" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A23" s="3" t="s">
         <v>30</v>
       </c>
@@ -1879,61 +1886,64 @@
       <c r="D23" s="1" t="s">
         <v>195</v>
       </c>
-      <c r="E23" s="3"/>
       <c r="F23" s="3"/>
       <c r="G23" s="3"/>
       <c r="H23" s="3"/>
-      <c r="I23" s="3" t="e">
+      <c r="I23" s="3"/>
+      <c r="J23" s="3" t="e">
         <f>INT((Table1[[#This Row],[current section]]/Table1[[#This Row],[total sections]])*100)&amp;"%"</f>
         <v>#DIV/0!</v>
       </c>
-      <c r="J23" s="3"/>
       <c r="K23" s="3"/>
-      <c r="L23" s="3" t="s">
+      <c r="L23" s="3"/>
+      <c r="M23" s="3" t="s">
         <v>119</v>
       </c>
-      <c r="M23" s="3" t="s">
+      <c r="N23" s="3" t="s">
         <v>120</v>
       </c>
-      <c r="N23" s="3" t="s">
+      <c r="O23" s="3" t="s">
         <v>121</v>
       </c>
     </row>
-    <row r="24" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A24" s="3">
+    <row r="24" spans="1:15" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A24" s="4">
         <v>2023</v>
       </c>
-      <c r="B24" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="C24" s="3" t="s">
+      <c r="B24" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="C24" s="4" t="s">
         <v>203</v>
       </c>
-      <c r="D24" s="1" t="s">
+      <c r="D24" s="6" t="s">
         <v>202</v>
       </c>
-      <c r="E24" s="7">
+      <c r="E24" s="6"/>
+      <c r="F24" s="5">
         <v>45117</v>
       </c>
-      <c r="F24" s="3"/>
-      <c r="G24" s="3">
+      <c r="G24" s="4"/>
+      <c r="H24" s="4">
         <v>3</v>
       </c>
-      <c r="H24" s="3">
+      <c r="I24" s="4">
         <v>26</v>
       </c>
-      <c r="I24" s="3" t="str">
+      <c r="J24" s="4" t="str">
         <f>INT((Table1[[#This Row],[current section]]/Table1[[#This Row],[total sections]])*100)&amp;"%"</f>
         <v>11%</v>
       </c>
-      <c r="J24" s="3"/>
-      <c r="K24" s="3"/>
-      <c r="L24" s="3">
-        <f>-L31</f>
+      <c r="K24" s="4"/>
+      <c r="L24" s="4" t="s">
+        <v>182</v>
+      </c>
+      <c r="M24" s="4">
+        <f>-M31</f>
         <v>0</v>
       </c>
-      <c r="M24" s="3"/>
-      <c r="N24" s="3" t="s">
+      <c r="N24" s="4"/>
+      <c r="O24" s="4" t="s">
         <v>146</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Changes made on Sun 07/23/2023 at 20:00:58.19 from PC Outside Home
</commit_message>
<xml_diff>
--- a/courses.xlsx
+++ b/courses.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26529"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24332"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Notes\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Notes\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{30B453AE-D6CC-4FCE-80E0-FFB144A4D2E2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D5FC4CA2-6E0B-402C-B370-4AE6A4DBEE32}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Videos" sheetId="2" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="329" uniqueCount="204">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="330" uniqueCount="205">
   <si>
     <t>duration</t>
   </si>
@@ -645,6 +645,9 @@
   </si>
   <si>
     <t>javascript</t>
+  </si>
+  <si>
+    <t>nested routes</t>
   </si>
 </sst>
 </file>
@@ -710,9 +713,6 @@
   </cellStyles>
   <dxfs count="16">
     <dxf>
-      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
@@ -742,6 +742,9 @@
     </dxf>
     <dxf>
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
@@ -782,19 +785,19 @@
     <tableColumn id="5" xr3:uid="{1DF95946-E7C7-4EEF-8374-81CBC97594F4}" name="plateform" dataDxfId="13"/>
     <tableColumn id="16" xr3:uid="{7DD00BB8-229C-4796-93B5-A5F7BFC9AADD}" name="main subject" dataDxfId="12"/>
     <tableColumn id="6" xr3:uid="{2A3E2F85-94E1-4138-8E16-ED7E54212EAF}" name="title" dataDxfId="11"/>
-    <tableColumn id="13" xr3:uid="{48F1BD13-876C-498D-A84D-9C92899C1E8A}" name="current lecture" dataDxfId="0"/>
-    <tableColumn id="7" xr3:uid="{FB48243A-6764-4A7F-A85C-D0443CC1E609}" name="started at" dataDxfId="10"/>
-    <tableColumn id="8" xr3:uid="{09458720-1B8F-4611-B7DD-C25E4166F7D2}" name="finished at" dataDxfId="9"/>
-    <tableColumn id="15" xr3:uid="{A97B4FA4-E868-4D80-9513-BBC292926A04}" name="current section" dataDxfId="8"/>
-    <tableColumn id="9" xr3:uid="{2E312EC2-08F1-4FEB-9E49-DA55B4987F10}" name="total sections" dataDxfId="7"/>
-    <tableColumn id="10" xr3:uid="{4D640820-9D97-4ABF-A25F-66744C2A935E}" name="progress" dataDxfId="6">
+    <tableColumn id="13" xr3:uid="{48F1BD13-876C-498D-A84D-9C92899C1E8A}" name="current lecture" dataDxfId="10"/>
+    <tableColumn id="7" xr3:uid="{FB48243A-6764-4A7F-A85C-D0443CC1E609}" name="started at" dataDxfId="9"/>
+    <tableColumn id="8" xr3:uid="{09458720-1B8F-4611-B7DD-C25E4166F7D2}" name="finished at" dataDxfId="8"/>
+    <tableColumn id="15" xr3:uid="{A97B4FA4-E868-4D80-9513-BBC292926A04}" name="current section" dataDxfId="7"/>
+    <tableColumn id="9" xr3:uid="{2E312EC2-08F1-4FEB-9E49-DA55B4987F10}" name="total sections" dataDxfId="6"/>
+    <tableColumn id="10" xr3:uid="{4D640820-9D97-4ABF-A25F-66744C2A935E}" name="progress" dataDxfId="5">
       <calculatedColumnFormula>INT((Table1[[#This Row],[current section]]/Table1[[#This Row],[total sections]])*100)&amp;"%"</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="11" xr3:uid="{9CB6E5D8-27A7-487B-816B-136D644B5102}" name="notes" dataDxfId="5"/>
-    <tableColumn id="12" xr3:uid="{93D4FB50-FA3D-49E2-94CB-397269CE9100}" name="has_git" dataDxfId="4"/>
-    <tableColumn id="1" xr3:uid="{BD9254B6-01AD-4D11-A881-3FE1B369F6A7}" name="duration" dataDxfId="3"/>
-    <tableColumn id="2" xr3:uid="{56126BA6-8875-4EF0-8824-A3CBC2A59B71}" name="description" dataDxfId="2"/>
-    <tableColumn id="3" xr3:uid="{C243BCA3-96B3-417B-A11B-C44FF935B7D2}" name="author" dataDxfId="1"/>
+    <tableColumn id="11" xr3:uid="{9CB6E5D8-27A7-487B-816B-136D644B5102}" name="notes" dataDxfId="4"/>
+    <tableColumn id="12" xr3:uid="{93D4FB50-FA3D-49E2-94CB-397269CE9100}" name="has_git" dataDxfId="3"/>
+    <tableColumn id="1" xr3:uid="{BD9254B6-01AD-4D11-A881-3FE1B369F6A7}" name="duration" dataDxfId="2"/>
+    <tableColumn id="2" xr3:uid="{56126BA6-8875-4EF0-8824-A3CBC2A59B71}" name="description" dataDxfId="1"/>
+    <tableColumn id="3" xr3:uid="{C243BCA3-96B3-417B-A11B-C44FF935B7D2}" name="author" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium16" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1110,27 +1113,27 @@
   <dimension ref="A1:O24"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G32" sqref="G32"/>
+      <selection activeCell="E15" sqref="E15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="7.85546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="10.85546875" customWidth="1"/>
+    <col min="1" max="1" width="7.88671875" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10.88671875" customWidth="1"/>
     <col min="3" max="3" width="14" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="60.7109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="30.42578125" style="1" customWidth="1"/>
-    <col min="6" max="6" width="12.85546875" customWidth="1"/>
-    <col min="7" max="7" width="11.28515625" customWidth="1"/>
-    <col min="8" max="8" width="6.5703125" customWidth="1"/>
-    <col min="9" max="9" width="6.85546875" customWidth="1"/>
-    <col min="10" max="10" width="9.7109375" customWidth="1"/>
-    <col min="13" max="13" width="13.42578125" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="105.28515625" customWidth="1"/>
-    <col min="15" max="15" width="34.7109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="60.6640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="30.44140625" style="1" customWidth="1"/>
+    <col min="6" max="6" width="12.88671875" customWidth="1"/>
+    <col min="7" max="7" width="11.33203125" customWidth="1"/>
+    <col min="8" max="8" width="6.5546875" customWidth="1"/>
+    <col min="9" max="9" width="6.88671875" customWidth="1"/>
+    <col min="10" max="10" width="9.6640625" customWidth="1"/>
+    <col min="13" max="13" width="13.44140625" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="105.33203125" customWidth="1"/>
+    <col min="15" max="15" width="34.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>160</v>
       </c>
@@ -1177,7 +1180,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A2" s="3" t="s">
         <v>79</v>
       </c>
@@ -1210,7 +1213,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="3" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A3" s="3" t="s">
         <v>20</v>
       </c>
@@ -1243,7 +1246,7 @@
         <v>136</v>
       </c>
     </row>
-    <row r="4" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A4" s="3" t="s">
         <v>30</v>
       </c>
@@ -1276,7 +1279,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="5" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A5" s="3" t="s">
         <v>35</v>
       </c>
@@ -1309,7 +1312,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="6" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A6" s="3" t="s">
         <v>25</v>
       </c>
@@ -1342,7 +1345,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="7" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A7" s="3" t="s">
         <v>10</v>
       </c>
@@ -1375,7 +1378,7 @@
         <v>159</v>
       </c>
     </row>
-    <row r="8" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A8" s="3" t="s">
         <v>35</v>
       </c>
@@ -1408,7 +1411,7 @@
         <v>124</v>
       </c>
     </row>
-    <row r="9" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A9" s="3" t="s">
         <v>35</v>
       </c>
@@ -1441,7 +1444,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="10" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A10" s="3" t="s">
         <v>25</v>
       </c>
@@ -1474,7 +1477,7 @@
         <v>124</v>
       </c>
     </row>
-    <row r="11" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A11" s="3" t="s">
         <v>25</v>
       </c>
@@ -1507,7 +1510,7 @@
         <v>124</v>
       </c>
     </row>
-    <row r="12" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A12" s="3" t="s">
         <v>25</v>
       </c>
@@ -1540,7 +1543,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="13" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A13" s="3" t="s">
         <v>79</v>
       </c>
@@ -1573,7 +1576,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="14" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A14" s="3" t="s">
         <v>25</v>
       </c>
@@ -1606,7 +1609,7 @@
         <v>136</v>
       </c>
     </row>
-    <row r="15" spans="1:15" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:15" s="2" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A15" s="4">
         <v>2023</v>
       </c>
@@ -1619,7 +1622,9 @@
       <c r="D15" s="6" t="s">
         <v>180</v>
       </c>
-      <c r="E15" s="6"/>
+      <c r="E15" s="6" t="s">
+        <v>204</v>
+      </c>
       <c r="F15" s="5" t="s">
         <v>181</v>
       </c>
@@ -1650,7 +1655,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="16" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A16" s="3" t="s">
         <v>25</v>
       </c>
@@ -1683,7 +1688,7 @@
         <v>108</v>
       </c>
     </row>
-    <row r="17" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A17" s="3">
         <v>2020</v>
       </c>
@@ -1716,7 +1721,7 @@
         <v>108</v>
       </c>
     </row>
-    <row r="18" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A18" s="3" t="s">
         <v>79</v>
       </c>
@@ -1749,7 +1754,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="19" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A19" s="3" t="s">
         <v>35</v>
       </c>
@@ -1782,7 +1787,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="20" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A20" s="3" t="s">
         <v>79</v>
       </c>
@@ -1813,7 +1818,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="21" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A21" s="3" t="s">
         <v>25</v>
       </c>
@@ -1844,7 +1849,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="22" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A22" s="3" t="s">
         <v>25</v>
       </c>
@@ -1875,7 +1880,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="23" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A23" s="3" t="s">
         <v>30</v>
       </c>
@@ -1906,7 +1911,7 @@
         <v>121</v>
       </c>
     </row>
-    <row r="24" spans="1:15" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:15" s="2" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A24" s="4">
         <v>2023</v>
       </c>
@@ -1963,22 +1968,22 @@
       <selection activeCell="G25" sqref="G25"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="9.7109375" customWidth="1"/>
-    <col min="2" max="2" width="101.85546875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="27.140625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="6.42578125" customWidth="1"/>
+    <col min="1" max="1" width="9.6640625" customWidth="1"/>
+    <col min="2" max="2" width="101.88671875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="27.109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="6.44140625" customWidth="1"/>
     <col min="5" max="5" width="11" customWidth="1"/>
-    <col min="6" max="6" width="49.5703125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="10.7109375" customWidth="1"/>
-    <col min="8" max="8" width="11.28515625" customWidth="1"/>
-    <col min="9" max="9" width="14.85546875" customWidth="1"/>
-    <col min="10" max="10" width="9.7109375" customWidth="1"/>
+    <col min="6" max="6" width="49.5546875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="10.6640625" customWidth="1"/>
+    <col min="8" max="8" width="11.33203125" customWidth="1"/>
+    <col min="9" max="9" width="14.88671875" customWidth="1"/>
+    <col min="10" max="10" width="9.6640625" customWidth="1"/>
     <col min="13" max="13" width="11" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -2019,7 +2024,7 @@
         <v>165</v>
       </c>
     </row>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>7</v>
       </c>
@@ -2042,7 +2047,7 @@
         <v>167</v>
       </c>
     </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>13</v>
       </c>
@@ -2065,7 +2070,7 @@
         <v>173</v>
       </c>
     </row>
-    <row r="4" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>17</v>
       </c>
@@ -2088,7 +2093,7 @@
         <v>173</v>
       </c>
     </row>
-    <row r="5" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>22</v>
       </c>
@@ -2111,7 +2116,7 @@
         <v>173</v>
       </c>
     </row>
-    <row r="6" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>27</v>
       </c>
@@ -2131,7 +2136,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="7" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>32</v>
       </c>
@@ -2154,7 +2159,7 @@
         <v>173</v>
       </c>
     </row>
-    <row r="8" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>37</v>
       </c>
@@ -2177,7 +2182,7 @@
         <v>174</v>
       </c>
     </row>
-    <row r="9" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>41</v>
       </c>
@@ -2200,7 +2205,7 @@
         <v>169</v>
       </c>
     </row>
-    <row r="10" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>45</v>
       </c>
@@ -2223,7 +2228,7 @@
         <v>172</v>
       </c>
     </row>
-    <row r="11" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>45</v>
       </c>
@@ -2246,7 +2251,7 @@
         <v>173</v>
       </c>
     </row>
-    <row r="12" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>52</v>
       </c>
@@ -2269,7 +2274,7 @@
         <v>167</v>
       </c>
     </row>
-    <row r="13" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>56</v>
       </c>
@@ -2289,7 +2294,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="14" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>17</v>
       </c>
@@ -2312,7 +2317,7 @@
         <v>169</v>
       </c>
     </row>
-    <row r="15" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>64</v>
       </c>
@@ -2335,7 +2340,7 @@
         <v>177</v>
       </c>
     </row>
-    <row r="16" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>68</v>
       </c>
@@ -2358,7 +2363,7 @@
         <v>173</v>
       </c>
     </row>
-    <row r="17" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
         <v>72</v>
       </c>
@@ -2378,7 +2383,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="18" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
         <v>76</v>
       </c>
@@ -2398,7 +2403,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="19" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
         <v>81</v>
       </c>
@@ -2418,7 +2423,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="20" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
         <v>85</v>
       </c>
@@ -2441,7 +2446,7 @@
         <v>172</v>
       </c>
     </row>
-    <row r="21" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
         <v>89</v>
       </c>
@@ -2464,7 +2469,7 @@
         <v>172</v>
       </c>
     </row>
-    <row r="22" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
         <v>93</v>
       </c>
@@ -2503,27 +2508,27 @@
       <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="68.28515625" customWidth="1"/>
+    <col min="1" max="1" width="68.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>199</v>
       </c>
     </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>198</v>
       </c>
     </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>200</v>
       </c>
     </row>
-    <row r="4" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>201</v>
       </c>

</xml_diff>

<commit_message>
Changes made on 24/07/2023 at  7:25:12,24 from PC Home
</commit_message>
<xml_diff>
--- a/courses.xlsx
+++ b/courses.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24332"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26529"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Notes\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Notes\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D5FC4CA2-6E0B-402C-B370-4AE6A4DBEE32}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{92D200A6-832E-4296-9424-3E4AD392AC4F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Videos" sheetId="2" r:id="rId1"/>
@@ -647,7 +647,7 @@
     <t>javascript</t>
   </si>
   <si>
-    <t>nested routes</t>
+    <t>introduction and demo</t>
   </si>
 </sst>
 </file>
@@ -1113,27 +1113,27 @@
   <dimension ref="A1:O24"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E15" sqref="E15"/>
+      <selection activeCell="E32" sqref="E32"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="7.88671875" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="10.88671875" customWidth="1"/>
+    <col min="1" max="1" width="7.85546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10.85546875" customWidth="1"/>
     <col min="3" max="3" width="14" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="60.6640625" style="1" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="30.44140625" style="1" customWidth="1"/>
-    <col min="6" max="6" width="12.88671875" customWidth="1"/>
-    <col min="7" max="7" width="11.33203125" customWidth="1"/>
-    <col min="8" max="8" width="6.5546875" customWidth="1"/>
-    <col min="9" max="9" width="6.88671875" customWidth="1"/>
-    <col min="10" max="10" width="9.6640625" customWidth="1"/>
-    <col min="13" max="13" width="13.44140625" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="105.33203125" customWidth="1"/>
-    <col min="15" max="15" width="34.6640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="60.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="30.42578125" style="1" customWidth="1"/>
+    <col min="6" max="6" width="12.85546875" customWidth="1"/>
+    <col min="7" max="7" width="11.28515625" customWidth="1"/>
+    <col min="8" max="8" width="6.5703125" customWidth="1"/>
+    <col min="9" max="9" width="6.85546875" customWidth="1"/>
+    <col min="10" max="10" width="9.7109375" customWidth="1"/>
+    <col min="13" max="13" width="13.42578125" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="105.28515625" customWidth="1"/>
+    <col min="15" max="15" width="34.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>160</v>
       </c>
@@ -1180,7 +1180,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
         <v>79</v>
       </c>
@@ -1213,7 +1213,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="3" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="s">
         <v>20</v>
       </c>
@@ -1246,7 +1246,7 @@
         <v>136</v>
       </c>
     </row>
-    <row r="4" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A4" s="3" t="s">
         <v>30</v>
       </c>
@@ -1279,7 +1279,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="5" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A5" s="3" t="s">
         <v>35</v>
       </c>
@@ -1312,7 +1312,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="6" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A6" s="3" t="s">
         <v>25</v>
       </c>
@@ -1345,7 +1345,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="7" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A7" s="3" t="s">
         <v>10</v>
       </c>
@@ -1378,7 +1378,7 @@
         <v>159</v>
       </c>
     </row>
-    <row r="8" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A8" s="3" t="s">
         <v>35</v>
       </c>
@@ -1411,7 +1411,7 @@
         <v>124</v>
       </c>
     </row>
-    <row r="9" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A9" s="3" t="s">
         <v>35</v>
       </c>
@@ -1444,7 +1444,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="10" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A10" s="3" t="s">
         <v>25</v>
       </c>
@@ -1477,7 +1477,7 @@
         <v>124</v>
       </c>
     </row>
-    <row r="11" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A11" s="3" t="s">
         <v>25</v>
       </c>
@@ -1510,7 +1510,7 @@
         <v>124</v>
       </c>
     </row>
-    <row r="12" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A12" s="3" t="s">
         <v>25</v>
       </c>
@@ -1543,7 +1543,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="13" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A13" s="3" t="s">
         <v>79</v>
       </c>
@@ -1576,7 +1576,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="14" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A14" s="3" t="s">
         <v>25</v>
       </c>
@@ -1609,7 +1609,7 @@
         <v>136</v>
       </c>
     </row>
-    <row r="15" spans="1:15" s="2" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:15" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A15" s="4">
         <v>2023</v>
       </c>
@@ -1630,14 +1630,14 @@
       </c>
       <c r="G15" s="4"/>
       <c r="H15" s="4">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="I15" s="4">
         <v>19</v>
       </c>
       <c r="J15" s="4" t="str">
         <f>INT((Table1[[#This Row],[current section]]/Table1[[#This Row],[total sections]])*100)&amp;"%"</f>
-        <v>42%</v>
+        <v>52%</v>
       </c>
       <c r="K15" s="4">
         <v>10</v>
@@ -1655,7 +1655,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="16" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A16" s="3" t="s">
         <v>25</v>
       </c>
@@ -1688,7 +1688,7 @@
         <v>108</v>
       </c>
     </row>
-    <row r="17" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A17" s="3">
         <v>2020</v>
       </c>
@@ -1721,7 +1721,7 @@
         <v>108</v>
       </c>
     </row>
-    <row r="18" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A18" s="3" t="s">
         <v>79</v>
       </c>
@@ -1754,7 +1754,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="19" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A19" s="3" t="s">
         <v>35</v>
       </c>
@@ -1787,7 +1787,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="20" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A20" s="3" t="s">
         <v>79</v>
       </c>
@@ -1818,7 +1818,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="21" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A21" s="3" t="s">
         <v>25</v>
       </c>
@@ -1849,7 +1849,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="22" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A22" s="3" t="s">
         <v>25</v>
       </c>
@@ -1880,7 +1880,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="23" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A23" s="3" t="s">
         <v>30</v>
       </c>
@@ -1911,7 +1911,7 @@
         <v>121</v>
       </c>
     </row>
-    <row r="24" spans="1:15" s="2" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:15" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A24" s="4">
         <v>2023</v>
       </c>
@@ -1968,22 +1968,22 @@
       <selection activeCell="G25" sqref="G25"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="9.6640625" customWidth="1"/>
-    <col min="2" max="2" width="101.88671875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="27.109375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="6.44140625" customWidth="1"/>
+    <col min="1" max="1" width="9.7109375" customWidth="1"/>
+    <col min="2" max="2" width="101.85546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="27.140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="6.42578125" customWidth="1"/>
     <col min="5" max="5" width="11" customWidth="1"/>
-    <col min="6" max="6" width="49.5546875" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="10.6640625" customWidth="1"/>
-    <col min="8" max="8" width="11.33203125" customWidth="1"/>
-    <col min="9" max="9" width="14.88671875" customWidth="1"/>
-    <col min="10" max="10" width="9.6640625" customWidth="1"/>
+    <col min="6" max="6" width="49.5703125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="10.7109375" customWidth="1"/>
+    <col min="8" max="8" width="11.28515625" customWidth="1"/>
+    <col min="9" max="9" width="14.85546875" customWidth="1"/>
+    <col min="10" max="10" width="9.7109375" customWidth="1"/>
     <col min="13" max="13" width="11" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -2024,7 +2024,7 @@
         <v>165</v>
       </c>
     </row>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>7</v>
       </c>
@@ -2047,7 +2047,7 @@
         <v>167</v>
       </c>
     </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>13</v>
       </c>
@@ -2070,7 +2070,7 @@
         <v>173</v>
       </c>
     </row>
-    <row r="4" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>17</v>
       </c>
@@ -2093,7 +2093,7 @@
         <v>173</v>
       </c>
     </row>
-    <row r="5" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>22</v>
       </c>
@@ -2116,7 +2116,7 @@
         <v>173</v>
       </c>
     </row>
-    <row r="6" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>27</v>
       </c>
@@ -2136,7 +2136,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="7" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>32</v>
       </c>
@@ -2159,7 +2159,7 @@
         <v>173</v>
       </c>
     </row>
-    <row r="8" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>37</v>
       </c>
@@ -2182,7 +2182,7 @@
         <v>174</v>
       </c>
     </row>
-    <row r="9" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>41</v>
       </c>
@@ -2205,7 +2205,7 @@
         <v>169</v>
       </c>
     </row>
-    <row r="10" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>45</v>
       </c>
@@ -2228,7 +2228,7 @@
         <v>172</v>
       </c>
     </row>
-    <row r="11" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>45</v>
       </c>
@@ -2251,7 +2251,7 @@
         <v>173</v>
       </c>
     </row>
-    <row r="12" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>52</v>
       </c>
@@ -2274,7 +2274,7 @@
         <v>167</v>
       </c>
     </row>
-    <row r="13" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>56</v>
       </c>
@@ -2294,7 +2294,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="14" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>17</v>
       </c>
@@ -2317,7 +2317,7 @@
         <v>169</v>
       </c>
     </row>
-    <row r="15" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>64</v>
       </c>
@@ -2340,7 +2340,7 @@
         <v>177</v>
       </c>
     </row>
-    <row r="16" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>68</v>
       </c>
@@ -2363,7 +2363,7 @@
         <v>173</v>
       </c>
     </row>
-    <row r="17" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>72</v>
       </c>
@@ -2383,7 +2383,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="18" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>76</v>
       </c>
@@ -2403,7 +2403,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="19" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>81</v>
       </c>
@@ -2423,7 +2423,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="20" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>85</v>
       </c>
@@ -2446,7 +2446,7 @@
         <v>172</v>
       </c>
     </row>
-    <row r="21" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>89</v>
       </c>
@@ -2469,7 +2469,7 @@
         <v>172</v>
       </c>
     </row>
-    <row r="22" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>93</v>
       </c>
@@ -2508,27 +2508,27 @@
       <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="68.33203125" customWidth="1"/>
+    <col min="1" max="1" width="68.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>199</v>
       </c>
     </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>198</v>
       </c>
     </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>200</v>
       </c>
     </row>
-    <row r="4" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>201</v>
       </c>

</xml_diff>

<commit_message>
Changes made on 30/07/2023 at 13:59:09,42 from PC Home
</commit_message>
<xml_diff>
--- a/courses.xlsx
+++ b/courses.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24332"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26529"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Notes\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Notes\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E65D7B66-228D-4300-8AE1-D2D91E185F67}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AFC49A20-A370-4D75-9CEF-95D43B88F601}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-1305" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Videos" sheetId="2" r:id="rId1"/>
@@ -647,7 +647,7 @@
     <t>javascript</t>
   </si>
   <si>
-    <t>responsive design</t>
+    <t>moviemate</t>
   </si>
 </sst>
 </file>
@@ -1113,27 +1113,27 @@
   <dimension ref="A1:O24"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E15" sqref="E15"/>
+      <selection activeCell="E28" sqref="E28"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="7.88671875" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="10.88671875" customWidth="1"/>
+    <col min="1" max="1" width="7.85546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10.85546875" customWidth="1"/>
     <col min="3" max="3" width="14" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="59" style="1" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="30.44140625" style="1" customWidth="1"/>
-    <col min="6" max="6" width="12.88671875" customWidth="1"/>
-    <col min="7" max="7" width="11.33203125" customWidth="1"/>
-    <col min="8" max="8" width="6.5546875" customWidth="1"/>
-    <col min="9" max="9" width="6.88671875" customWidth="1"/>
-    <col min="10" max="10" width="9.6640625" customWidth="1"/>
-    <col min="13" max="13" width="13.44140625" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="105.33203125" customWidth="1"/>
-    <col min="15" max="15" width="34.6640625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="30.42578125" style="1" customWidth="1"/>
+    <col min="6" max="6" width="12.85546875" customWidth="1"/>
+    <col min="7" max="7" width="11.28515625" customWidth="1"/>
+    <col min="8" max="8" width="6.5703125" customWidth="1"/>
+    <col min="9" max="9" width="6.85546875" customWidth="1"/>
+    <col min="10" max="10" width="9.7109375" customWidth="1"/>
+    <col min="13" max="13" width="13.42578125" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="105.28515625" customWidth="1"/>
+    <col min="15" max="15" width="34.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>160</v>
       </c>
@@ -1180,7 +1180,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
         <v>79</v>
       </c>
@@ -1213,7 +1213,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="3" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="s">
         <v>20</v>
       </c>
@@ -1246,7 +1246,7 @@
         <v>136</v>
       </c>
     </row>
-    <row r="4" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A4" s="3" t="s">
         <v>30</v>
       </c>
@@ -1279,7 +1279,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="5" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A5" s="3" t="s">
         <v>35</v>
       </c>
@@ -1312,7 +1312,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="6" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A6" s="3" t="s">
         <v>25</v>
       </c>
@@ -1345,7 +1345,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="7" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A7" s="3" t="s">
         <v>10</v>
       </c>
@@ -1378,7 +1378,7 @@
         <v>159</v>
       </c>
     </row>
-    <row r="8" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A8" s="3" t="s">
         <v>35</v>
       </c>
@@ -1411,7 +1411,7 @@
         <v>124</v>
       </c>
     </row>
-    <row r="9" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A9" s="3" t="s">
         <v>35</v>
       </c>
@@ -1444,7 +1444,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="10" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A10" s="3" t="s">
         <v>25</v>
       </c>
@@ -1477,7 +1477,7 @@
         <v>124</v>
       </c>
     </row>
-    <row r="11" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A11" s="3" t="s">
         <v>25</v>
       </c>
@@ -1510,7 +1510,7 @@
         <v>124</v>
       </c>
     </row>
-    <row r="12" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A12" s="3" t="s">
         <v>25</v>
       </c>
@@ -1543,7 +1543,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="13" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A13" s="3" t="s">
         <v>79</v>
       </c>
@@ -1576,7 +1576,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="14" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A14" s="3" t="s">
         <v>25</v>
       </c>
@@ -1609,7 +1609,7 @@
         <v>136</v>
       </c>
     </row>
-    <row r="15" spans="1:15" s="2" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:15" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A15" s="4">
         <v>2023</v>
       </c>
@@ -1630,14 +1630,14 @@
       </c>
       <c r="G15" s="4"/>
       <c r="H15" s="4">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="I15" s="4">
         <v>19</v>
       </c>
       <c r="J15" s="4" t="str">
         <f>INT((Table1[[#This Row],[current section]]/Table1[[#This Row],[total sections]])*100)&amp;"%"</f>
-        <v>52%</v>
+        <v>57%</v>
       </c>
       <c r="K15" s="4">
         <v>10</v>
@@ -1655,7 +1655,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="16" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A16" s="3" t="s">
         <v>25</v>
       </c>
@@ -1688,7 +1688,7 @@
         <v>108</v>
       </c>
     </row>
-    <row r="17" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A17" s="3">
         <v>2020</v>
       </c>
@@ -1721,7 +1721,7 @@
         <v>108</v>
       </c>
     </row>
-    <row r="18" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A18" s="3" t="s">
         <v>79</v>
       </c>
@@ -1754,7 +1754,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="19" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A19" s="3" t="s">
         <v>35</v>
       </c>
@@ -1787,7 +1787,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="20" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A20" s="3" t="s">
         <v>79</v>
       </c>
@@ -1818,7 +1818,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="21" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A21" s="3" t="s">
         <v>25</v>
       </c>
@@ -1849,7 +1849,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="22" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A22" s="3" t="s">
         <v>25</v>
       </c>
@@ -1880,7 +1880,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="23" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A23" s="3" t="s">
         <v>30</v>
       </c>
@@ -1911,7 +1911,7 @@
         <v>121</v>
       </c>
     </row>
-    <row r="24" spans="1:15" s="2" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:15" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A24" s="4">
         <v>2023</v>
       </c>
@@ -1968,22 +1968,22 @@
       <selection activeCell="F5" sqref="F5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="9.6640625" customWidth="1"/>
-    <col min="2" max="2" width="101.88671875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="27.109375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="6.44140625" customWidth="1"/>
+    <col min="1" max="1" width="9.7109375" customWidth="1"/>
+    <col min="2" max="2" width="101.85546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="27.140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="6.42578125" customWidth="1"/>
     <col min="5" max="5" width="11" customWidth="1"/>
-    <col min="6" max="6" width="49.5546875" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="10.6640625" customWidth="1"/>
-    <col min="8" max="8" width="11.33203125" customWidth="1"/>
-    <col min="9" max="9" width="14.88671875" customWidth="1"/>
-    <col min="10" max="10" width="9.6640625" customWidth="1"/>
+    <col min="6" max="6" width="49.5703125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="10.7109375" customWidth="1"/>
+    <col min="8" max="8" width="11.28515625" customWidth="1"/>
+    <col min="9" max="9" width="14.85546875" customWidth="1"/>
+    <col min="10" max="10" width="9.7109375" customWidth="1"/>
     <col min="13" max="13" width="11" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -2024,7 +2024,7 @@
         <v>165</v>
       </c>
     </row>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>7</v>
       </c>
@@ -2047,7 +2047,7 @@
         <v>167</v>
       </c>
     </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>13</v>
       </c>
@@ -2070,7 +2070,7 @@
         <v>173</v>
       </c>
     </row>
-    <row r="4" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>17</v>
       </c>
@@ -2093,7 +2093,7 @@
         <v>173</v>
       </c>
     </row>
-    <row r="5" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>22</v>
       </c>
@@ -2116,7 +2116,7 @@
         <v>173</v>
       </c>
     </row>
-    <row r="6" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>27</v>
       </c>
@@ -2136,7 +2136,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="7" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>32</v>
       </c>
@@ -2159,7 +2159,7 @@
         <v>173</v>
       </c>
     </row>
-    <row r="8" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>37</v>
       </c>
@@ -2182,7 +2182,7 @@
         <v>174</v>
       </c>
     </row>
-    <row r="9" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>41</v>
       </c>
@@ -2205,7 +2205,7 @@
         <v>169</v>
       </c>
     </row>
-    <row r="10" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>45</v>
       </c>
@@ -2228,7 +2228,7 @@
         <v>172</v>
       </c>
     </row>
-    <row r="11" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>45</v>
       </c>
@@ -2251,7 +2251,7 @@
         <v>173</v>
       </c>
     </row>
-    <row r="12" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>52</v>
       </c>
@@ -2274,7 +2274,7 @@
         <v>167</v>
       </c>
     </row>
-    <row r="13" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>56</v>
       </c>
@@ -2294,7 +2294,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="14" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>17</v>
       </c>
@@ -2317,7 +2317,7 @@
         <v>169</v>
       </c>
     </row>
-    <row r="15" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>64</v>
       </c>
@@ -2340,7 +2340,7 @@
         <v>177</v>
       </c>
     </row>
-    <row r="16" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>68</v>
       </c>
@@ -2363,7 +2363,7 @@
         <v>173</v>
       </c>
     </row>
-    <row r="17" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>72</v>
       </c>
@@ -2383,7 +2383,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="18" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>76</v>
       </c>
@@ -2403,7 +2403,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="19" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>81</v>
       </c>
@@ -2423,7 +2423,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="20" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>85</v>
       </c>
@@ -2446,7 +2446,7 @@
         <v>172</v>
       </c>
     </row>
-    <row r="21" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>89</v>
       </c>
@@ -2469,7 +2469,7 @@
         <v>172</v>
       </c>
     </row>
-    <row r="22" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>93</v>
       </c>
@@ -2508,27 +2508,27 @@
       <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="68.33203125" customWidth="1"/>
+    <col min="1" max="1" width="68.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>199</v>
       </c>
     </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>198</v>
       </c>
     </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>200</v>
       </c>
     </row>
-    <row r="4" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>201</v>
       </c>

</xml_diff>

<commit_message>
Changes made on Wed 08/23/2023 at 18:45:23.46 from PC Outside Home
</commit_message>
<xml_diff>
--- a/courses.xlsx
+++ b/courses.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26529"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24332"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Notes\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Notes\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AFC49A20-A370-4D75-9CEF-95D43B88F601}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F8D64A6D-626D-4798-9178-56EAD8A14DE7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Videos" sheetId="2" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="330" uniqueCount="205">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="335" uniqueCount="209">
   <si>
     <t>duration</t>
   </si>
@@ -648,6 +648,18 @@
   </si>
   <si>
     <t>moviemate</t>
+  </si>
+  <si>
+    <t>github</t>
+  </si>
+  <si>
+    <t>Learning github actions for devops</t>
+  </si>
+  <si>
+    <t>adding self hosted runner</t>
+  </si>
+  <si>
+    <t>no</t>
   </si>
 </sst>
 </file>
@@ -663,7 +675,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -673,6 +685,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FF92D050"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.39997558519241921"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -689,7 +707,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -706,6 +724,18 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -775,8 +805,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{F5801A2D-4A6C-4794-B5C6-BD54C875A28D}" name="Table1" displayName="Table1" ref="A1:O24" totalsRowShown="0" dataDxfId="15">
-  <autoFilter ref="A1:O24" xr:uid="{F5801A2D-4A6C-4794-B5C6-BD54C875A28D}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{F5801A2D-4A6C-4794-B5C6-BD54C875A28D}" name="Table1" displayName="Table1" ref="A1:O25" totalsRowShown="0" dataDxfId="15">
+  <autoFilter ref="A1:O25" xr:uid="{F5801A2D-4A6C-4794-B5C6-BD54C875A28D}"/>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:O23">
     <sortCondition ref="C1:C23"/>
   </sortState>
@@ -1110,10 +1140,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:O24"/>
+  <dimension ref="A1:O25"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E28" sqref="E28"/>
+      <selection activeCell="M24" sqref="M24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1125,8 +1155,8 @@
     <col min="5" max="5" width="30.42578125" style="1" customWidth="1"/>
     <col min="6" max="6" width="12.85546875" customWidth="1"/>
     <col min="7" max="7" width="11.28515625" customWidth="1"/>
-    <col min="8" max="8" width="6.5703125" customWidth="1"/>
-    <col min="9" max="9" width="6.85546875" customWidth="1"/>
+    <col min="8" max="8" width="16.7109375" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="15.140625" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="9.7109375" customWidth="1"/>
     <col min="13" max="13" width="13.42578125" bestFit="1" customWidth="1"/>
     <col min="14" max="14" width="105.28515625" customWidth="1"/>
@@ -1912,43 +1942,81 @@
       </c>
     </row>
     <row r="24" spans="1:15" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A24" s="4">
+      <c r="A24" s="7">
         <v>2023</v>
       </c>
-      <c r="B24" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="C24" s="4" t="s">
+      <c r="B24" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="C24" s="7" t="s">
+        <v>205</v>
+      </c>
+      <c r="D24" s="8" t="s">
+        <v>206</v>
+      </c>
+      <c r="E24" s="8" t="s">
+        <v>207</v>
+      </c>
+      <c r="F24" s="9">
+        <v>45130</v>
+      </c>
+      <c r="G24" s="7"/>
+      <c r="H24" s="7">
+        <v>3</v>
+      </c>
+      <c r="I24" s="7">
+        <v>6</v>
+      </c>
+      <c r="J24" s="10" t="str">
+        <f>INT((Table1[[#This Row],[current section]]/Table1[[#This Row],[total sections]])*100)&amp;"%"</f>
+        <v>50%</v>
+      </c>
+      <c r="K24" s="7"/>
+      <c r="L24" s="7" t="s">
+        <v>208</v>
+      </c>
+      <c r="M24" s="7"/>
+      <c r="N24" s="7"/>
+      <c r="O24" s="7"/>
+    </row>
+    <row r="25" spans="1:15" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A25" s="4">
+        <v>2023</v>
+      </c>
+      <c r="B25" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="C25" s="4" t="s">
         <v>203</v>
       </c>
-      <c r="D24" s="6" t="s">
+      <c r="D25" s="6" t="s">
         <v>202</v>
       </c>
-      <c r="E24" s="6"/>
-      <c r="F24" s="5">
+      <c r="E25" s="6"/>
+      <c r="F25" s="5">
         <v>45117</v>
       </c>
-      <c r="G24" s="4"/>
-      <c r="H24" s="4">
+      <c r="G25" s="4"/>
+      <c r="H25" s="4">
         <v>3</v>
       </c>
-      <c r="I24" s="4">
+      <c r="I25" s="4">
         <v>26</v>
       </c>
-      <c r="J24" s="4" t="str">
+      <c r="J25" s="4" t="str">
         <f>INT((Table1[[#This Row],[current section]]/Table1[[#This Row],[total sections]])*100)&amp;"%"</f>
         <v>11%</v>
       </c>
-      <c r="K24" s="4"/>
-      <c r="L24" s="4" t="s">
+      <c r="K25" s="4"/>
+      <c r="L25" s="4" t="s">
         <v>182</v>
       </c>
-      <c r="M24" s="4">
-        <f>-M31</f>
+      <c r="M25" s="4">
+        <f>-M32</f>
         <v>0</v>
       </c>
-      <c r="N24" s="4"/>
-      <c r="O24" s="4" t="s">
+      <c r="N25" s="4"/>
+      <c r="O25" s="4" t="s">
         <v>146</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Changes made on Thu 08/24/2023 at 11:37:54.12 from PC Outside Home
</commit_message>
<xml_diff>
--- a/courses.xlsx
+++ b/courses.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Notes\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F8D64A6D-626D-4798-9178-56EAD8A14DE7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E482345E-2E90-4C0B-A507-AC50A461DCF8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Videos" sheetId="2" r:id="rId1"/>
@@ -1143,27 +1143,27 @@
   <dimension ref="A1:O25"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="M24" sqref="M24"/>
+      <selection activeCell="I28" sqref="I28"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="7.85546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="10.85546875" customWidth="1"/>
+    <col min="1" max="1" width="7.88671875" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10.88671875" customWidth="1"/>
     <col min="3" max="3" width="14" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="59" style="1" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="30.42578125" style="1" customWidth="1"/>
-    <col min="6" max="6" width="12.85546875" customWidth="1"/>
-    <col min="7" max="7" width="11.28515625" customWidth="1"/>
-    <col min="8" max="8" width="16.7109375" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="15.140625" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="9.7109375" customWidth="1"/>
-    <col min="13" max="13" width="13.42578125" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="105.28515625" customWidth="1"/>
-    <col min="15" max="15" width="34.7109375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="30.44140625" style="1" customWidth="1"/>
+    <col min="6" max="6" width="12.88671875" customWidth="1"/>
+    <col min="7" max="7" width="11.33203125" customWidth="1"/>
+    <col min="8" max="8" width="16.6640625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="15.109375" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="9.6640625" customWidth="1"/>
+    <col min="13" max="13" width="13.44140625" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="105.33203125" customWidth="1"/>
+    <col min="15" max="15" width="34.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>160</v>
       </c>
@@ -1210,7 +1210,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A2" s="3" t="s">
         <v>79</v>
       </c>
@@ -1243,7 +1243,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="3" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A3" s="3" t="s">
         <v>20</v>
       </c>
@@ -1276,7 +1276,7 @@
         <v>136</v>
       </c>
     </row>
-    <row r="4" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A4" s="3" t="s">
         <v>30</v>
       </c>
@@ -1309,7 +1309,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="5" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A5" s="3" t="s">
         <v>35</v>
       </c>
@@ -1342,7 +1342,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="6" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A6" s="3" t="s">
         <v>25</v>
       </c>
@@ -1375,7 +1375,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="7" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A7" s="3" t="s">
         <v>10</v>
       </c>
@@ -1408,7 +1408,7 @@
         <v>159</v>
       </c>
     </row>
-    <row r="8" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A8" s="3" t="s">
         <v>35</v>
       </c>
@@ -1441,7 +1441,7 @@
         <v>124</v>
       </c>
     </row>
-    <row r="9" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A9" s="3" t="s">
         <v>35</v>
       </c>
@@ -1474,7 +1474,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="10" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A10" s="3" t="s">
         <v>25</v>
       </c>
@@ -1507,7 +1507,7 @@
         <v>124</v>
       </c>
     </row>
-    <row r="11" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A11" s="3" t="s">
         <v>25</v>
       </c>
@@ -1540,7 +1540,7 @@
         <v>124</v>
       </c>
     </row>
-    <row r="12" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A12" s="3" t="s">
         <v>25</v>
       </c>
@@ -1573,7 +1573,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="13" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A13" s="3" t="s">
         <v>79</v>
       </c>
@@ -1606,7 +1606,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="14" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A14" s="3" t="s">
         <v>25</v>
       </c>
@@ -1639,7 +1639,7 @@
         <v>136</v>
       </c>
     </row>
-    <row r="15" spans="1:15" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:15" s="2" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A15" s="4">
         <v>2023</v>
       </c>
@@ -1685,7 +1685,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="16" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A16" s="3" t="s">
         <v>25</v>
       </c>
@@ -1718,7 +1718,7 @@
         <v>108</v>
       </c>
     </row>
-    <row r="17" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A17" s="3">
         <v>2020</v>
       </c>
@@ -1751,7 +1751,7 @@
         <v>108</v>
       </c>
     </row>
-    <row r="18" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A18" s="3" t="s">
         <v>79</v>
       </c>
@@ -1784,7 +1784,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="19" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A19" s="3" t="s">
         <v>35</v>
       </c>
@@ -1817,7 +1817,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="20" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A20" s="3" t="s">
         <v>79</v>
       </c>
@@ -1848,7 +1848,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="21" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A21" s="3" t="s">
         <v>25</v>
       </c>
@@ -1879,7 +1879,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="22" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A22" s="3" t="s">
         <v>25</v>
       </c>
@@ -1910,7 +1910,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="23" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A23" s="3" t="s">
         <v>30</v>
       </c>
@@ -1941,7 +1941,7 @@
         <v>121</v>
       </c>
     </row>
-    <row r="24" spans="1:15" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:15" s="2" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A24" s="7">
         <v>2023</v>
       </c>
@@ -1962,14 +1962,14 @@
       </c>
       <c r="G24" s="7"/>
       <c r="H24" s="7">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="I24" s="7">
         <v>6</v>
       </c>
       <c r="J24" s="10" t="str">
         <f>INT((Table1[[#This Row],[current section]]/Table1[[#This Row],[total sections]])*100)&amp;"%"</f>
-        <v>50%</v>
+        <v>83%</v>
       </c>
       <c r="K24" s="7"/>
       <c r="L24" s="7" t="s">
@@ -1979,7 +1979,7 @@
       <c r="N24" s="7"/>
       <c r="O24" s="7"/>
     </row>
-    <row r="25" spans="1:15" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:15" s="2" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A25" s="4">
         <v>2023</v>
       </c>
@@ -2036,22 +2036,22 @@
       <selection activeCell="F5" sqref="F5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="9.7109375" customWidth="1"/>
-    <col min="2" max="2" width="101.85546875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="27.140625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="6.42578125" customWidth="1"/>
+    <col min="1" max="1" width="9.6640625" customWidth="1"/>
+    <col min="2" max="2" width="101.88671875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="27.109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="6.44140625" customWidth="1"/>
     <col min="5" max="5" width="11" customWidth="1"/>
-    <col min="6" max="6" width="49.5703125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="10.7109375" customWidth="1"/>
-    <col min="8" max="8" width="11.28515625" customWidth="1"/>
-    <col min="9" max="9" width="14.85546875" customWidth="1"/>
-    <col min="10" max="10" width="9.7109375" customWidth="1"/>
+    <col min="6" max="6" width="49.5546875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="10.6640625" customWidth="1"/>
+    <col min="8" max="8" width="11.33203125" customWidth="1"/>
+    <col min="9" max="9" width="14.88671875" customWidth="1"/>
+    <col min="10" max="10" width="9.6640625" customWidth="1"/>
     <col min="13" max="13" width="11" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -2092,7 +2092,7 @@
         <v>165</v>
       </c>
     </row>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>7</v>
       </c>
@@ -2115,7 +2115,7 @@
         <v>167</v>
       </c>
     </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>13</v>
       </c>
@@ -2138,7 +2138,7 @@
         <v>173</v>
       </c>
     </row>
-    <row r="4" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>17</v>
       </c>
@@ -2161,7 +2161,7 @@
         <v>173</v>
       </c>
     </row>
-    <row r="5" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>22</v>
       </c>
@@ -2184,7 +2184,7 @@
         <v>173</v>
       </c>
     </row>
-    <row r="6" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>27</v>
       </c>
@@ -2204,7 +2204,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="7" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>32</v>
       </c>
@@ -2227,7 +2227,7 @@
         <v>173</v>
       </c>
     </row>
-    <row r="8" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>37</v>
       </c>
@@ -2250,7 +2250,7 @@
         <v>174</v>
       </c>
     </row>
-    <row r="9" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>41</v>
       </c>
@@ -2273,7 +2273,7 @@
         <v>169</v>
       </c>
     </row>
-    <row r="10" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>45</v>
       </c>
@@ -2296,7 +2296,7 @@
         <v>172</v>
       </c>
     </row>
-    <row r="11" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>45</v>
       </c>
@@ -2319,7 +2319,7 @@
         <v>173</v>
       </c>
     </row>
-    <row r="12" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>52</v>
       </c>
@@ -2342,7 +2342,7 @@
         <v>167</v>
       </c>
     </row>
-    <row r="13" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>56</v>
       </c>
@@ -2362,7 +2362,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="14" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>17</v>
       </c>
@@ -2385,7 +2385,7 @@
         <v>169</v>
       </c>
     </row>
-    <row r="15" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>64</v>
       </c>
@@ -2408,7 +2408,7 @@
         <v>177</v>
       </c>
     </row>
-    <row r="16" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>68</v>
       </c>
@@ -2431,7 +2431,7 @@
         <v>173</v>
       </c>
     </row>
-    <row r="17" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
         <v>72</v>
       </c>
@@ -2451,7 +2451,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="18" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
         <v>76</v>
       </c>
@@ -2471,7 +2471,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="19" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
         <v>81</v>
       </c>
@@ -2491,7 +2491,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="20" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
         <v>85</v>
       </c>
@@ -2514,7 +2514,7 @@
         <v>172</v>
       </c>
     </row>
-    <row r="21" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
         <v>89</v>
       </c>
@@ -2537,7 +2537,7 @@
         <v>172</v>
       </c>
     </row>
-    <row r="22" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
         <v>93</v>
       </c>
@@ -2576,27 +2576,27 @@
       <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="68.28515625" customWidth="1"/>
+    <col min="1" max="1" width="68.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>199</v>
       </c>
     </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>198</v>
       </c>
     </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>200</v>
       </c>
     </row>
-    <row r="4" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>201</v>
       </c>

</xml_diff>

<commit_message>
Changes made on Thu 09/07/2023 at  7:32:00.96 from PC Outside Home
</commit_message>
<xml_diff>
--- a/courses.xlsx
+++ b/courses.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26731"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24332"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Notes\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Notes\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5230027E-C591-408E-9772-CC7C12217A10}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6DA043BD-286A-4516-89E5-50F76AAEE2A9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Videos" sheetId="2" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="359" uniqueCount="226">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="360" uniqueCount="227">
   <si>
     <t>duration</t>
   </si>
@@ -711,6 +711,9 @@
   </si>
   <si>
     <t>Priority</t>
+  </si>
+  <si>
+    <t>Learn Ethical Hacking From A-Z: Beginner To Expert Course</t>
   </si>
 </sst>
 </file>
@@ -776,7 +779,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="3">
+  <borders count="4">
     <border>
       <left/>
       <right/>
@@ -808,11 +811,24 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="27">
+  <cellXfs count="31">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -878,6 +894,18 @@
     <xf numFmtId="9" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1240,8 +1268,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{F5801A2D-4A6C-4794-B5C6-BD54C875A28D}" name="Table1" displayName="Table1" ref="A1:N35" totalsRowShown="0" dataDxfId="14">
-  <autoFilter ref="A1:N35" xr:uid="{F5801A2D-4A6C-4794-B5C6-BD54C875A28D}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{F5801A2D-4A6C-4794-B5C6-BD54C875A28D}" name="Table1" displayName="Table1" ref="A1:N36" totalsRowShown="0" dataDxfId="14">
+  <autoFilter ref="A1:N36" xr:uid="{F5801A2D-4A6C-4794-B5C6-BD54C875A28D}"/>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:N25">
     <sortCondition ref="D1:D25"/>
   </sortState>
@@ -1579,28 +1607,28 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:AY42"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="H1" workbookViewId="0">
-      <selection activeCell="O1" sqref="O1:O1048576"/>
+    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="F36" sqref="F36"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="7.85546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="10.85546875" customWidth="1"/>
-    <col min="3" max="3" width="6.28515625" customWidth="1"/>
+    <col min="1" max="1" width="7.88671875" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10.88671875" customWidth="1"/>
+    <col min="3" max="3" width="6.33203125" customWidth="1"/>
     <col min="4" max="4" width="14" customWidth="1"/>
-    <col min="5" max="5" width="9.85546875" style="10" customWidth="1"/>
-    <col min="6" max="6" width="62.140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="24.140625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="11.7109375" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="16.7109375" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="15.140625" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="12.7109375" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="109.7109375" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="38.42578125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="9.88671875" style="10" customWidth="1"/>
+    <col min="6" max="6" width="62.109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="24.109375" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="11.6640625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="16.6640625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="15.109375" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="12.6640625" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="109.6640625" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="38.44140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:51" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:51" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>154</v>
       </c>
@@ -1644,7 +1672,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:51" s="3" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:51" s="3" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A2" s="12" t="s">
         <v>74</v>
       </c>
@@ -1677,7 +1705,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="3" spans="1:51" s="3" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:51" s="3" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A3" s="12" t="s">
         <v>20</v>
       </c>
@@ -1710,7 +1738,7 @@
         <v>131</v>
       </c>
     </row>
-    <row r="4" spans="1:51" s="3" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:51" s="3" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A4" s="12" t="s">
         <v>30</v>
       </c>
@@ -1779,7 +1807,7 @@
       <c r="AX4"/>
       <c r="AY4"/>
     </row>
-    <row r="5" spans="1:51" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:51" x14ac:dyDescent="0.3">
       <c r="A5" s="16" t="s">
         <v>35</v>
       </c>
@@ -1812,7 +1840,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="6" spans="1:51" s="5" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:51" s="5" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A6" s="19" t="s">
         <v>25</v>
       </c>
@@ -1881,7 +1909,7 @@
       <c r="AX6"/>
       <c r="AY6"/>
     </row>
-    <row r="7" spans="1:51" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:51" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A7" s="16" t="s">
         <v>10</v>
       </c>
@@ -1920,7 +1948,7 @@
       </c>
       <c r="U7" s="1"/>
     </row>
-    <row r="8" spans="1:51" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:51" x14ac:dyDescent="0.3">
       <c r="A8" s="16" t="s">
         <v>25</v>
       </c>
@@ -1959,7 +1987,7 @@
       </c>
       <c r="U8" s="1"/>
     </row>
-    <row r="9" spans="1:51" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:51" x14ac:dyDescent="0.3">
       <c r="A9" s="16" t="s">
         <v>35</v>
       </c>
@@ -1998,7 +2026,7 @@
       </c>
       <c r="U9" s="1"/>
     </row>
-    <row r="10" spans="1:51" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:51" x14ac:dyDescent="0.3">
       <c r="A10" s="16" t="s">
         <v>35</v>
       </c>
@@ -2037,7 +2065,7 @@
       </c>
       <c r="U10" s="1"/>
     </row>
-    <row r="11" spans="1:51" s="7" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:51" s="7" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A11" s="22">
         <v>2023</v>
       </c>
@@ -2108,7 +2136,7 @@
       <c r="AX11"/>
       <c r="AY11"/>
     </row>
-    <row r="12" spans="1:51" s="7" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:51" s="7" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A12" s="22">
         <v>2023</v>
       </c>
@@ -2182,7 +2210,7 @@
       <c r="AX12"/>
       <c r="AY12"/>
     </row>
-    <row r="13" spans="1:51" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:51" x14ac:dyDescent="0.3">
       <c r="A13" s="16" t="s">
         <v>25</v>
       </c>
@@ -2217,7 +2245,7 @@
       <c r="R13" s="1"/>
       <c r="U13" s="1"/>
     </row>
-    <row r="14" spans="1:51" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:51" x14ac:dyDescent="0.3">
       <c r="A14" s="16" t="s">
         <v>25</v>
       </c>
@@ -2252,7 +2280,7 @@
       <c r="R14" s="1"/>
       <c r="U14" s="1"/>
     </row>
-    <row r="15" spans="1:51" s="5" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:51" s="5" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A15" s="19" t="s">
         <v>74</v>
       </c>
@@ -2321,7 +2349,7 @@
       <c r="AX15"/>
       <c r="AY15"/>
     </row>
-    <row r="16" spans="1:51" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:51" x14ac:dyDescent="0.3">
       <c r="A16" s="16" t="s">
         <v>25</v>
       </c>
@@ -2354,7 +2382,7 @@
         <v>131</v>
       </c>
     </row>
-    <row r="17" spans="1:51" s="7" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:51" s="7" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A17" s="22">
         <v>2023</v>
       </c>
@@ -2431,7 +2459,7 @@
       <c r="AX17"/>
       <c r="AY17"/>
     </row>
-    <row r="18" spans="1:51" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:51" x14ac:dyDescent="0.3">
       <c r="A18" s="16" t="s">
         <v>25</v>
       </c>
@@ -2464,7 +2492,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="19" spans="1:51" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:51" x14ac:dyDescent="0.3">
       <c r="A19" s="16" t="s">
         <v>74</v>
       </c>
@@ -2497,7 +2525,7 @@
         <v>125</v>
       </c>
     </row>
-    <row r="20" spans="1:51" s="3" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:51" s="3" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A20" s="12">
         <v>2020</v>
       </c>
@@ -2566,7 +2594,7 @@
       <c r="AX20"/>
       <c r="AY20"/>
     </row>
-    <row r="21" spans="1:51" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:51" x14ac:dyDescent="0.3">
       <c r="A21" s="16" t="s">
         <v>35</v>
       </c>
@@ -2599,7 +2627,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="22" spans="1:51" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:51" x14ac:dyDescent="0.3">
       <c r="A22" s="16" t="s">
         <v>25</v>
       </c>
@@ -2630,7 +2658,7 @@
         <v>141</v>
       </c>
     </row>
-    <row r="23" spans="1:51" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:51" x14ac:dyDescent="0.3">
       <c r="A23" s="16" t="s">
         <v>25</v>
       </c>
@@ -2661,7 +2689,7 @@
         <v>108</v>
       </c>
     </row>
-    <row r="24" spans="1:51" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:51" s="2" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A24" s="16" t="s">
         <v>74</v>
       </c>
@@ -2728,7 +2756,7 @@
       <c r="AX24"/>
       <c r="AY24"/>
     </row>
-    <row r="25" spans="1:51" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:51" s="4" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A25" s="16" t="s">
         <v>30</v>
       </c>
@@ -2795,7 +2823,7 @@
       <c r="AX25"/>
       <c r="AY25"/>
     </row>
-    <row r="26" spans="1:51" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:51" x14ac:dyDescent="0.3">
       <c r="A26" s="16"/>
       <c r="B26" s="16" t="s">
         <v>215</v>
@@ -2820,7 +2848,7 @@
       <c r="M26" s="16"/>
       <c r="N26" s="16"/>
     </row>
-    <row r="27" spans="1:51" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:51" x14ac:dyDescent="0.3">
       <c r="A27" s="16"/>
       <c r="B27" s="16" t="s">
         <v>215</v>
@@ -2844,7 +2872,7 @@
       <c r="M27" s="16"/>
       <c r="N27" s="16"/>
     </row>
-    <row r="28" spans="1:51" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:51" x14ac:dyDescent="0.3">
       <c r="A28" s="16"/>
       <c r="B28" s="16" t="s">
         <v>215</v>
@@ -2868,7 +2896,7 @@
       <c r="M28" s="16"/>
       <c r="N28" s="16"/>
     </row>
-    <row r="29" spans="1:51" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:51" x14ac:dyDescent="0.3">
       <c r="A29" s="16"/>
       <c r="B29" s="16" t="s">
         <v>215</v>
@@ -2892,7 +2920,7 @@
       <c r="M29" s="16"/>
       <c r="N29" s="16"/>
     </row>
-    <row r="30" spans="1:51" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:51" x14ac:dyDescent="0.3">
       <c r="A30" s="16"/>
       <c r="B30" s="16" t="s">
         <v>215</v>
@@ -2916,7 +2944,7 @@
       <c r="M30" s="16"/>
       <c r="N30" s="16"/>
     </row>
-    <row r="31" spans="1:51" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:51" x14ac:dyDescent="0.3">
       <c r="A31" s="16"/>
       <c r="B31" s="16" t="s">
         <v>215</v>
@@ -2941,7 +2969,7 @@
       <c r="M31" s="16"/>
       <c r="N31" s="16"/>
     </row>
-    <row r="32" spans="1:51" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:51" x14ac:dyDescent="0.3">
       <c r="A32" s="16"/>
       <c r="B32" s="16" t="s">
         <v>215</v>
@@ -2965,7 +2993,7 @@
       <c r="M32" s="16"/>
       <c r="N32" s="16"/>
     </row>
-    <row r="33" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A33" s="16"/>
       <c r="B33" s="16" t="s">
         <v>215</v>
@@ -2990,7 +3018,7 @@
       <c r="M33" s="16"/>
       <c r="N33" s="16"/>
     </row>
-    <row r="34" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A34" s="16"/>
       <c r="B34" s="16" t="s">
         <v>215</v>
@@ -3014,7 +3042,7 @@
       <c r="M34" s="16"/>
       <c r="N34" s="16"/>
     </row>
-    <row r="35" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A35" s="16"/>
       <c r="B35" s="16" t="s">
         <v>215</v>
@@ -3038,13 +3066,34 @@
       <c r="M35" s="16"/>
       <c r="N35" s="16"/>
     </row>
-    <row r="37" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A36" s="27"/>
+      <c r="B36" s="27"/>
+      <c r="C36" s="27"/>
+      <c r="D36" s="27"/>
+      <c r="E36" s="28" t="e">
+        <f>INT((Table1[[#This Row],[current section]]/Table1[[#This Row],[total sections]])*100)&amp;"%"</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="F36" s="30" t="s">
+        <v>226</v>
+      </c>
+      <c r="G36" s="29"/>
+      <c r="H36" s="27"/>
+      <c r="I36" s="27"/>
+      <c r="J36" s="27"/>
+      <c r="K36" s="27"/>
+      <c r="L36" s="27"/>
+      <c r="M36" s="27"/>
+      <c r="N36" s="27"/>
+    </row>
+    <row r="37" spans="1:14" x14ac:dyDescent="0.3">
       <c r="E37" s="11" t="str">
         <f>PROPER(F2)</f>
         <v>Architecting Reactive Angular Applications With Redux A…</v>
       </c>
     </row>
-    <row r="42" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:14" x14ac:dyDescent="0.3">
       <c r="E42" s="10" t="str">
         <f>PROPER(F16)</f>
         <v>React - The Complete Guide (Includes Hooks, React Route...</v>
@@ -3063,25 +3112,25 @@
   <dimension ref="A1:M21"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C30" sqref="C30"/>
+      <selection activeCell="F10" sqref="F10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="9.7109375" customWidth="1"/>
-    <col min="2" max="2" width="101.85546875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="27.140625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="6.42578125" customWidth="1"/>
+    <col min="1" max="1" width="9.6640625" customWidth="1"/>
+    <col min="2" max="2" width="101.88671875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="27.109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="6.44140625" customWidth="1"/>
     <col min="5" max="5" width="11" customWidth="1"/>
-    <col min="6" max="6" width="49.5703125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="10.7109375" customWidth="1"/>
-    <col min="8" max="8" width="11.28515625" customWidth="1"/>
-    <col min="9" max="9" width="14.85546875" customWidth="1"/>
-    <col min="10" max="10" width="9.7109375" customWidth="1"/>
+    <col min="6" max="6" width="49.5546875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="10.6640625" customWidth="1"/>
+    <col min="8" max="8" width="11.33203125" customWidth="1"/>
+    <col min="9" max="9" width="14.88671875" customWidth="1"/>
+    <col min="10" max="10" width="9.6640625" customWidth="1"/>
     <col min="13" max="13" width="11" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -3122,7 +3171,7 @@
         <v>159</v>
       </c>
     </row>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>13</v>
       </c>
@@ -3145,7 +3194,7 @@
         <v>167</v>
       </c>
     </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>17</v>
       </c>
@@ -3168,7 +3217,7 @@
         <v>167</v>
       </c>
     </row>
-    <row r="4" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>22</v>
       </c>
@@ -3191,7 +3240,7 @@
         <v>167</v>
       </c>
     </row>
-    <row r="5" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>32</v>
       </c>
@@ -3214,7 +3263,7 @@
         <v>167</v>
       </c>
     </row>
-    <row r="6" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>45</v>
       </c>
@@ -3237,7 +3286,7 @@
         <v>167</v>
       </c>
     </row>
-    <row r="7" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>63</v>
       </c>
@@ -3260,7 +3309,7 @@
         <v>167</v>
       </c>
     </row>
-    <row r="8" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>41</v>
       </c>
@@ -3283,7 +3332,7 @@
         <v>163</v>
       </c>
     </row>
-    <row r="9" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>17</v>
       </c>
@@ -3306,7 +3355,7 @@
         <v>163</v>
       </c>
     </row>
-    <row r="10" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>37</v>
       </c>
@@ -3329,7 +3378,7 @@
         <v>168</v>
       </c>
     </row>
-    <row r="11" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>45</v>
       </c>
@@ -3352,7 +3401,7 @@
         <v>166</v>
       </c>
     </row>
-    <row r="12" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>80</v>
       </c>
@@ -3375,7 +3424,7 @@
         <v>166</v>
       </c>
     </row>
-    <row r="13" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>84</v>
       </c>
@@ -3398,7 +3447,7 @@
         <v>166</v>
       </c>
     </row>
-    <row r="14" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>88</v>
       </c>
@@ -3421,7 +3470,7 @@
         <v>166</v>
       </c>
     </row>
-    <row r="15" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>7</v>
       </c>
@@ -3444,7 +3493,7 @@
         <v>161</v>
       </c>
     </row>
-    <row r="16" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>52</v>
       </c>
@@ -3467,7 +3516,7 @@
         <v>161</v>
       </c>
     </row>
-    <row r="17" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
         <v>59</v>
       </c>
@@ -3490,7 +3539,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="18" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
         <v>27</v>
       </c>
@@ -3510,7 +3559,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="19" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
         <v>67</v>
       </c>
@@ -3530,7 +3579,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="20" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
         <v>71</v>
       </c>
@@ -3550,7 +3599,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="21" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
         <v>76</v>
       </c>
@@ -3583,30 +3632,30 @@
   <dimension ref="A1:A4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A4" sqref="A4"/>
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="68.28515625" customWidth="1"/>
+    <col min="1" max="1" width="68.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>191</v>
       </c>
     </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>190</v>
       </c>
     </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>192</v>
       </c>
     </row>
-    <row r="4" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>193</v>
       </c>

</xml_diff>

<commit_message>
Changes made on 07/09/2023 at  7:32:49,56 from PC Home
</commit_message>
<xml_diff>
--- a/courses.xlsx
+++ b/courses.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Notes\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5230027E-C591-408E-9772-CC7C12217A10}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2616AEA1-154F-42EC-AF4F-90F924E09C03}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -812,7 +812,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="27">
+  <cellXfs count="21">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -829,27 +829,15 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -857,17 +845,11 @@
     <xf numFmtId="0" fontId="0" fillId="5" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -1242,8 +1224,8 @@
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{F5801A2D-4A6C-4794-B5C6-BD54C875A28D}" name="Table1" displayName="Table1" ref="A1:N35" totalsRowShown="0" dataDxfId="14">
   <autoFilter ref="A1:N35" xr:uid="{F5801A2D-4A6C-4794-B5C6-BD54C875A28D}"/>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:N25">
-    <sortCondition ref="D1:D25"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:N35">
+    <sortCondition ref="A1:A35"/>
   </sortState>
   <tableColumns count="14">
     <tableColumn id="4" xr3:uid="{4A213850-DE4B-4FE6-B4B5-91277FE7FF66}" name="year" dataDxfId="13"/>
@@ -1579,8 +1561,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:AY42"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="H1" workbookViewId="0">
-      <selection activeCell="O1" sqref="O1:O1048576"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F9" sqref="F8:F9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1589,7 +1571,7 @@
     <col min="2" max="2" width="10.85546875" customWidth="1"/>
     <col min="3" max="3" width="6.28515625" customWidth="1"/>
     <col min="4" max="4" width="14" customWidth="1"/>
-    <col min="5" max="5" width="9.85546875" style="10" customWidth="1"/>
+    <col min="5" max="5" width="9.85546875" style="1" customWidth="1"/>
     <col min="6" max="6" width="62.140625" style="1" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="24.140625" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="11.7109375" bestFit="1" customWidth="1"/>
@@ -1616,7 +1598,7 @@
       <c r="E1" t="s">
         <v>224</v>
       </c>
-      <c r="F1" s="10" t="s">
+      <c r="F1" s="1" t="s">
         <v>156</v>
       </c>
       <c r="G1" s="1" t="s">
@@ -1645,103 +1627,83 @@
       </c>
     </row>
     <row r="2" spans="1:51" s="3" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="12" t="s">
-        <v>74</v>
-      </c>
-      <c r="B2" s="12" t="s">
-        <v>11</v>
-      </c>
-      <c r="C2" s="12"/>
-      <c r="D2" s="12" t="s">
-        <v>167</v>
-      </c>
-      <c r="E2" s="12" t="e">
+      <c r="A2" s="13">
+        <v>2015</v>
+      </c>
+      <c r="B2" s="13" t="s">
+        <v>215</v>
+      </c>
+      <c r="C2" s="13"/>
+      <c r="D2" s="13" t="s">
+        <v>219</v>
+      </c>
+      <c r="E2" s="20">
+        <v>0.46</v>
+      </c>
+      <c r="F2" s="14" t="s">
+        <v>208</v>
+      </c>
+      <c r="G2" s="14"/>
+      <c r="H2" s="13"/>
+      <c r="I2" s="13"/>
+      <c r="J2" s="13"/>
+      <c r="K2" s="13"/>
+      <c r="L2" s="13"/>
+      <c r="M2" s="13"/>
+      <c r="N2" s="13"/>
+    </row>
+    <row r="3" spans="1:51" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="13">
+        <v>2015</v>
+      </c>
+      <c r="B3" s="13" t="s">
+        <v>215</v>
+      </c>
+      <c r="C3" s="13"/>
+      <c r="D3" s="13" t="s">
+        <v>221</v>
+      </c>
+      <c r="E3" s="13" t="e">
         <f>INT((Table1[[#This Row],[current section]]/Table1[[#This Row],[total sections]])*100)&amp;"%"</f>
         <v>#DIV/0!</v>
       </c>
-      <c r="F2" s="13" t="s">
-        <v>202</v>
-      </c>
-      <c r="G2" s="14"/>
-      <c r="H2" s="12"/>
-      <c r="I2" s="12"/>
-      <c r="J2" s="12"/>
-      <c r="K2" s="12"/>
-      <c r="L2" s="12" t="s">
-        <v>143</v>
-      </c>
-      <c r="M2" s="12" t="s">
-        <v>144</v>
-      </c>
-      <c r="N2" s="12" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="3" spans="1:51" s="3" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="12" t="s">
-        <v>20</v>
-      </c>
-      <c r="B3" s="12" t="s">
-        <v>11</v>
-      </c>
-      <c r="C3" s="12"/>
-      <c r="D3" s="12" t="s">
-        <v>167</v>
-      </c>
-      <c r="E3" s="12" t="e">
-        <f>INT((Table1[[#This Row],[current section]]/Table1[[#This Row],[total sections]])*100)&amp;"%"</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="F3" s="13" t="s">
-        <v>132</v>
+      <c r="F3" s="14" t="s">
+        <v>212</v>
       </c>
       <c r="G3" s="14"/>
-      <c r="H3" s="12"/>
-      <c r="I3" s="12"/>
-      <c r="J3" s="12"/>
-      <c r="K3" s="12"/>
-      <c r="L3" s="12" t="s">
-        <v>129</v>
-      </c>
-      <c r="M3" s="12" t="s">
-        <v>130</v>
-      </c>
-      <c r="N3" s="12" t="s">
-        <v>131</v>
-      </c>
+      <c r="H3" s="13"/>
+      <c r="I3" s="13"/>
+      <c r="J3" s="13"/>
+      <c r="K3" s="13"/>
+      <c r="L3" s="13"/>
+      <c r="M3" s="13"/>
+      <c r="N3" s="13"/>
     </row>
     <row r="4" spans="1:51" s="3" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="12" t="s">
-        <v>30</v>
-      </c>
-      <c r="B4" s="12" t="s">
-        <v>11</v>
-      </c>
-      <c r="C4" s="12"/>
-      <c r="D4" s="12" t="s">
-        <v>167</v>
-      </c>
-      <c r="E4" s="12" t="e">
-        <f>INT((Table1[[#This Row],[current section]]/Table1[[#This Row],[total sections]])*100)&amp;"%"</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="F4" s="15" t="s">
-        <v>177</v>
-      </c>
-      <c r="G4" s="12"/>
-      <c r="H4" s="12"/>
-      <c r="I4" s="12"/>
-      <c r="J4" s="12"/>
-      <c r="K4" s="12"/>
-      <c r="L4" s="12" t="s">
-        <v>92</v>
-      </c>
-      <c r="M4" s="12" t="s">
-        <v>93</v>
-      </c>
-      <c r="N4" s="12" t="s">
-        <v>94</v>
-      </c>
+      <c r="A4" s="13">
+        <v>2016</v>
+      </c>
+      <c r="B4" s="13" t="s">
+        <v>215</v>
+      </c>
+      <c r="C4" s="13"/>
+      <c r="D4" s="13" t="s">
+        <v>218</v>
+      </c>
+      <c r="E4" s="20">
+        <v>0.7</v>
+      </c>
+      <c r="F4" s="14" t="s">
+        <v>207</v>
+      </c>
+      <c r="G4" s="14"/>
+      <c r="H4" s="13"/>
+      <c r="I4" s="13"/>
+      <c r="J4" s="13"/>
+      <c r="K4" s="13"/>
+      <c r="L4" s="13"/>
+      <c r="M4" s="13"/>
+      <c r="N4" s="13"/>
       <c r="P4"/>
       <c r="Q4"/>
       <c r="R4"/>
@@ -1780,70 +1742,56 @@
       <c r="AY4"/>
     </row>
     <row r="5" spans="1:51" x14ac:dyDescent="0.25">
-      <c r="A5" s="16" t="s">
-        <v>35</v>
-      </c>
-      <c r="B5" s="16" t="s">
-        <v>11</v>
-      </c>
-      <c r="C5" s="16"/>
-      <c r="D5" s="16" t="s">
-        <v>169</v>
-      </c>
-      <c r="E5" s="16" t="e">
-        <f>INT((Table1[[#This Row],[current section]]/Table1[[#This Row],[total sections]])*100)&amp;"%"</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="F5" s="17" t="s">
-        <v>189</v>
-      </c>
-      <c r="G5" s="18"/>
-      <c r="H5" s="16"/>
-      <c r="I5" s="16"/>
-      <c r="J5" s="16"/>
-      <c r="K5" s="16"/>
-      <c r="L5" s="16" t="s">
-        <v>98</v>
-      </c>
-      <c r="M5" s="16" t="s">
-        <v>99</v>
-      </c>
-      <c r="N5" s="16" t="s">
-        <v>100</v>
-      </c>
+      <c r="A5" s="13">
+        <v>2016</v>
+      </c>
+      <c r="B5" s="13" t="s">
+        <v>215</v>
+      </c>
+      <c r="C5" s="13"/>
+      <c r="D5" s="13" t="s">
+        <v>220</v>
+      </c>
+      <c r="E5" s="20">
+        <v>0.78</v>
+      </c>
+      <c r="F5" s="14" t="s">
+        <v>209</v>
+      </c>
+      <c r="G5" s="14"/>
+      <c r="H5" s="13"/>
+      <c r="I5" s="13"/>
+      <c r="J5" s="13"/>
+      <c r="K5" s="13"/>
+      <c r="L5" s="13"/>
+      <c r="M5" s="13"/>
+      <c r="N5" s="13"/>
     </row>
     <row r="6" spans="1:51" s="5" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="19" t="s">
-        <v>25</v>
-      </c>
-      <c r="B6" s="19" t="s">
-        <v>11</v>
-      </c>
-      <c r="C6" s="19"/>
-      <c r="D6" s="19" t="s">
+      <c r="A6" s="13">
+        <v>2016</v>
+      </c>
+      <c r="B6" s="13" t="s">
+        <v>215</v>
+      </c>
+      <c r="C6" s="13"/>
+      <c r="D6" s="13" t="s">
         <v>160</v>
       </c>
-      <c r="E6" s="19" t="e">
-        <f>INT((Table1[[#This Row],[current section]]/Table1[[#This Row],[total sections]])*100)&amp;"%"</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="F6" s="20" t="s">
-        <v>188</v>
-      </c>
-      <c r="G6" s="21"/>
-      <c r="H6" s="19"/>
-      <c r="I6" s="19"/>
-      <c r="J6" s="19"/>
-      <c r="K6" s="19"/>
-      <c r="L6" s="19" t="s">
-        <v>126</v>
-      </c>
-      <c r="M6" s="19" t="s">
-        <v>127</v>
-      </c>
-      <c r="N6" s="19" t="s">
-        <v>128</v>
-      </c>
+      <c r="E6" s="20">
+        <v>0.25</v>
+      </c>
+      <c r="F6" s="14" t="s">
+        <v>216</v>
+      </c>
+      <c r="G6" s="14"/>
+      <c r="H6" s="13"/>
+      <c r="I6" s="13"/>
+      <c r="J6" s="13"/>
+      <c r="K6" s="13"/>
+      <c r="L6" s="13"/>
+      <c r="M6" s="13"/>
+      <c r="N6" s="13"/>
       <c r="P6"/>
       <c r="Q6"/>
       <c r="R6" s="1"/>
@@ -1882,37 +1830,31 @@
       <c r="AY6"/>
     </row>
     <row r="7" spans="1:51" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="16" t="s">
-        <v>10</v>
-      </c>
-      <c r="B7" s="16" t="s">
-        <v>11</v>
-      </c>
-      <c r="C7" s="16"/>
-      <c r="D7" s="16" t="s">
-        <v>165</v>
-      </c>
-      <c r="E7" s="16" t="e">
+      <c r="A7" s="13">
+        <v>2018</v>
+      </c>
+      <c r="B7" s="13" t="s">
+        <v>215</v>
+      </c>
+      <c r="C7" s="13"/>
+      <c r="D7" s="13" t="s">
+        <v>200</v>
+      </c>
+      <c r="E7" s="13" t="e">
         <f>INT((Table1[[#This Row],[current section]]/Table1[[#This Row],[total sections]])*100)&amp;"%"</f>
         <v>#DIV/0!</v>
       </c>
-      <c r="F7" s="17" t="s">
-        <v>178</v>
-      </c>
-      <c r="G7" s="18"/>
-      <c r="H7" s="16"/>
-      <c r="I7" s="16"/>
-      <c r="J7" s="16"/>
-      <c r="K7" s="16"/>
-      <c r="L7" s="16" t="s">
-        <v>151</v>
-      </c>
-      <c r="M7" s="16" t="s">
-        <v>152</v>
-      </c>
-      <c r="N7" s="16" t="s">
-        <v>153</v>
-      </c>
+      <c r="F7" s="14" t="s">
+        <v>214</v>
+      </c>
+      <c r="G7" s="14"/>
+      <c r="H7" s="13"/>
+      <c r="I7" s="13"/>
+      <c r="J7" s="13"/>
+      <c r="K7" s="13"/>
+      <c r="L7" s="13"/>
+      <c r="M7" s="13"/>
+      <c r="N7" s="13"/>
       <c r="R7" s="1"/>
       <c r="S7" s="9"/>
       <c r="T7" t="s">
@@ -1921,37 +1863,30 @@
       <c r="U7" s="1"/>
     </row>
     <row r="8" spans="1:51" x14ac:dyDescent="0.25">
-      <c r="A8" s="16" t="s">
-        <v>25</v>
-      </c>
-      <c r="B8" s="16" t="s">
-        <v>11</v>
-      </c>
-      <c r="C8" s="16"/>
-      <c r="D8" s="16" t="s">
-        <v>163</v>
-      </c>
-      <c r="E8" s="16" t="e">
-        <f>INT((Table1[[#This Row],[current section]]/Table1[[#This Row],[total sections]])*100)&amp;"%"</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="F8" s="17" t="s">
-        <v>180</v>
-      </c>
-      <c r="G8" s="18"/>
-      <c r="H8" s="16"/>
-      <c r="I8" s="16"/>
-      <c r="J8" s="16"/>
-      <c r="K8" s="16"/>
-      <c r="L8" s="16" t="s">
-        <v>135</v>
-      </c>
-      <c r="M8" s="16" t="s">
-        <v>136</v>
-      </c>
-      <c r="N8" s="16" t="s">
-        <v>119</v>
-      </c>
+      <c r="A8" s="13">
+        <v>2018</v>
+      </c>
+      <c r="B8" s="13" t="s">
+        <v>215</v>
+      </c>
+      <c r="C8" s="13"/>
+      <c r="D8" s="13" t="s">
+        <v>217</v>
+      </c>
+      <c r="E8" s="20">
+        <v>0.15</v>
+      </c>
+      <c r="F8" s="14" t="s">
+        <v>206</v>
+      </c>
+      <c r="G8" s="14"/>
+      <c r="H8" s="13"/>
+      <c r="I8" s="13"/>
+      <c r="J8" s="13"/>
+      <c r="K8" s="13"/>
+      <c r="L8" s="13"/>
+      <c r="M8" s="13"/>
+      <c r="N8" s="13"/>
       <c r="R8" s="1"/>
       <c r="S8" s="6"/>
       <c r="T8" t="s">
@@ -1960,37 +1895,30 @@
       <c r="U8" s="1"/>
     </row>
     <row r="9" spans="1:51" x14ac:dyDescent="0.25">
-      <c r="A9" s="16" t="s">
-        <v>35</v>
-      </c>
-      <c r="B9" s="16" t="s">
-        <v>11</v>
-      </c>
-      <c r="C9" s="16"/>
-      <c r="D9" s="16" t="s">
-        <v>163</v>
-      </c>
-      <c r="E9" s="16" t="e">
-        <f>INT((Table1[[#This Row],[current section]]/Table1[[#This Row],[total sections]])*100)&amp;"%"</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="F9" s="17" t="s">
-        <v>120</v>
-      </c>
-      <c r="G9" s="18"/>
-      <c r="H9" s="16"/>
-      <c r="I9" s="16"/>
-      <c r="J9" s="16"/>
-      <c r="K9" s="16"/>
-      <c r="L9" s="16" t="s">
-        <v>117</v>
-      </c>
-      <c r="M9" s="16" t="s">
-        <v>118</v>
-      </c>
-      <c r="N9" s="16" t="s">
-        <v>119</v>
-      </c>
+      <c r="A9" s="13">
+        <v>2018</v>
+      </c>
+      <c r="B9" s="13" t="s">
+        <v>215</v>
+      </c>
+      <c r="C9" s="13"/>
+      <c r="D9" s="13" t="s">
+        <v>223</v>
+      </c>
+      <c r="E9" s="20">
+        <v>0.86</v>
+      </c>
+      <c r="F9" s="14" t="s">
+        <v>213</v>
+      </c>
+      <c r="G9" s="14"/>
+      <c r="H9" s="13"/>
+      <c r="I9" s="13"/>
+      <c r="J9" s="13"/>
+      <c r="K9" s="13"/>
+      <c r="L9" s="13"/>
+      <c r="M9" s="13"/>
+      <c r="N9" s="13"/>
       <c r="R9" s="1"/>
       <c r="S9" s="5"/>
       <c r="T9" t="s">
@@ -1999,36 +1927,36 @@
       <c r="U9" s="1"/>
     </row>
     <row r="10" spans="1:51" x14ac:dyDescent="0.25">
-      <c r="A10" s="16" t="s">
-        <v>35</v>
-      </c>
-      <c r="B10" s="16" t="s">
-        <v>11</v>
-      </c>
-      <c r="C10" s="16"/>
-      <c r="D10" s="16" t="s">
-        <v>163</v>
-      </c>
-      <c r="E10" s="16" t="e">
+      <c r="A10" s="11">
+        <v>2020</v>
+      </c>
+      <c r="B10" s="11" t="s">
+        <v>11</v>
+      </c>
+      <c r="C10" s="11"/>
+      <c r="D10" s="11" t="s">
+        <v>164</v>
+      </c>
+      <c r="E10" s="11" t="e">
         <f>INT((Table1[[#This Row],[current section]]/Table1[[#This Row],[total sections]])*100)&amp;"%"</f>
         <v>#DIV/0!</v>
       </c>
-      <c r="F10" s="17" t="s">
-        <v>179</v>
-      </c>
-      <c r="G10" s="18"/>
-      <c r="H10" s="16"/>
-      <c r="I10" s="16"/>
-      <c r="J10" s="16"/>
-      <c r="K10" s="16"/>
-      <c r="L10" s="16" t="s">
-        <v>137</v>
-      </c>
-      <c r="M10" s="16" t="s">
-        <v>138</v>
-      </c>
-      <c r="N10" s="16" t="s">
-        <v>100</v>
+      <c r="F10" s="12" t="s">
+        <v>184</v>
+      </c>
+      <c r="G10" s="12"/>
+      <c r="H10" s="11"/>
+      <c r="I10" s="11"/>
+      <c r="J10" s="11"/>
+      <c r="K10" s="11"/>
+      <c r="L10" s="11" t="s">
+        <v>104</v>
+      </c>
+      <c r="M10" s="11" t="s">
+        <v>105</v>
+      </c>
+      <c r="N10" s="11" t="s">
+        <v>103</v>
       </c>
       <c r="R10" s="1"/>
       <c r="S10" s="8"/>
@@ -2038,39 +1966,30 @@
       <c r="U10" s="1"/>
     </row>
     <row r="11" spans="1:51" s="7" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="22">
-        <v>2023</v>
-      </c>
-      <c r="B11" s="22" t="s">
-        <v>11</v>
-      </c>
-      <c r="C11" s="22"/>
-      <c r="D11" s="22" t="s">
-        <v>197</v>
-      </c>
-      <c r="E11" s="22" t="str">
-        <f>INT((Table1[[#This Row],[current section]]/Table1[[#This Row],[total sections]])*100)&amp;"%"</f>
-        <v>83%</v>
-      </c>
-      <c r="F11" s="23" t="s">
-        <v>198</v>
-      </c>
-      <c r="G11" s="24" t="s">
-        <v>199</v>
-      </c>
-      <c r="H11" s="25">
-        <v>45130</v>
-      </c>
-      <c r="I11" s="22"/>
-      <c r="J11" s="22">
-        <v>5</v>
-      </c>
-      <c r="K11" s="22">
-        <v>6</v>
-      </c>
-      <c r="L11" s="22"/>
-      <c r="M11" s="22"/>
-      <c r="N11" s="22"/>
+      <c r="A11" s="13">
+        <v>2020</v>
+      </c>
+      <c r="B11" s="13" t="s">
+        <v>215</v>
+      </c>
+      <c r="C11" s="13"/>
+      <c r="D11" s="13" t="s">
+        <v>166</v>
+      </c>
+      <c r="E11" s="20">
+        <v>0.15</v>
+      </c>
+      <c r="F11" s="14" t="s">
+        <v>210</v>
+      </c>
+      <c r="G11" s="14"/>
+      <c r="H11" s="13"/>
+      <c r="I11" s="13"/>
+      <c r="J11" s="13"/>
+      <c r="K11" s="13"/>
+      <c r="L11" s="13"/>
+      <c r="M11" s="13"/>
+      <c r="N11" s="13"/>
       <c r="P11"/>
       <c r="Q11"/>
       <c r="R11" s="1"/>
@@ -2109,42 +2028,31 @@
       <c r="AY11"/>
     </row>
     <row r="12" spans="1:51" s="7" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="22">
-        <v>2023</v>
-      </c>
-      <c r="B12" s="22" t="s">
-        <v>11</v>
-      </c>
-      <c r="C12" s="22"/>
-      <c r="D12" s="22" t="s">
-        <v>195</v>
-      </c>
-      <c r="E12" s="22" t="str">
+      <c r="A12" s="13">
+        <v>2021</v>
+      </c>
+      <c r="B12" s="13" t="s">
+        <v>215</v>
+      </c>
+      <c r="C12" s="13"/>
+      <c r="D12" s="13" t="s">
+        <v>222</v>
+      </c>
+      <c r="E12" s="13" t="e">
         <f>INT((Table1[[#This Row],[current section]]/Table1[[#This Row],[total sections]])*100)&amp;"%"</f>
-        <v>11%</v>
-      </c>
-      <c r="F12" s="23" t="s">
-        <v>194</v>
-      </c>
-      <c r="G12" s="24"/>
-      <c r="H12" s="25">
-        <v>45117</v>
-      </c>
-      <c r="I12" s="22"/>
-      <c r="J12" s="22">
-        <v>3</v>
-      </c>
-      <c r="K12" s="22">
-        <v>26</v>
-      </c>
-      <c r="L12" s="22" t="e">
-        <f>-L19</f>
-        <v>#VALUE!</v>
-      </c>
-      <c r="M12" s="22"/>
-      <c r="N12" s="22" t="s">
-        <v>141</v>
-      </c>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="F12" s="14" t="s">
+        <v>211</v>
+      </c>
+      <c r="G12" s="14"/>
+      <c r="H12" s="13"/>
+      <c r="I12" s="13"/>
+      <c r="J12" s="13"/>
+      <c r="K12" s="13"/>
+      <c r="L12" s="13"/>
+      <c r="M12" s="13"/>
+      <c r="N12" s="13"/>
       <c r="P12"/>
       <c r="Q12"/>
       <c r="R12" s="1"/>
@@ -2183,106 +2091,121 @@
       <c r="AY12"/>
     </row>
     <row r="13" spans="1:51" x14ac:dyDescent="0.25">
-      <c r="A13" s="16" t="s">
-        <v>25</v>
-      </c>
-      <c r="B13" s="16" t="s">
-        <v>11</v>
-      </c>
-      <c r="C13" s="16"/>
-      <c r="D13" s="16" t="s">
-        <v>168</v>
-      </c>
-      <c r="E13" s="16" t="e">
+      <c r="A13" s="17">
+        <v>2023</v>
+      </c>
+      <c r="B13" s="17" t="s">
+        <v>11</v>
+      </c>
+      <c r="C13" s="17"/>
+      <c r="D13" s="17" t="s">
+        <v>197</v>
+      </c>
+      <c r="E13" s="17" t="str">
         <f>INT((Table1[[#This Row],[current section]]/Table1[[#This Row],[total sections]])*100)&amp;"%"</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="F13" s="17" t="s">
-        <v>181</v>
-      </c>
-      <c r="G13" s="18"/>
-      <c r="H13" s="16"/>
-      <c r="I13" s="16"/>
-      <c r="J13" s="16"/>
-      <c r="K13" s="16"/>
-      <c r="L13" s="16" t="s">
-        <v>133</v>
-      </c>
-      <c r="M13" s="16" t="s">
-        <v>134</v>
-      </c>
-      <c r="N13" s="16" t="s">
-        <v>119</v>
-      </c>
+        <v>83%</v>
+      </c>
+      <c r="F13" s="18" t="s">
+        <v>198</v>
+      </c>
+      <c r="G13" s="18" t="s">
+        <v>199</v>
+      </c>
+      <c r="H13" s="19">
+        <v>45130</v>
+      </c>
+      <c r="I13" s="17"/>
+      <c r="J13" s="17">
+        <v>5</v>
+      </c>
+      <c r="K13" s="17">
+        <v>6</v>
+      </c>
+      <c r="L13" s="17"/>
+      <c r="M13" s="17"/>
+      <c r="N13" s="17"/>
       <c r="R13" s="1"/>
       <c r="U13" s="1"/>
     </row>
     <row r="14" spans="1:51" x14ac:dyDescent="0.25">
-      <c r="A14" s="16" t="s">
-        <v>25</v>
-      </c>
-      <c r="B14" s="16" t="s">
-        <v>11</v>
-      </c>
-      <c r="C14" s="16"/>
-      <c r="D14" s="16" t="s">
-        <v>162</v>
-      </c>
-      <c r="E14" s="16" t="e">
+      <c r="A14" s="17">
+        <v>2023</v>
+      </c>
+      <c r="B14" s="17" t="s">
+        <v>11</v>
+      </c>
+      <c r="C14" s="17"/>
+      <c r="D14" s="17" t="s">
+        <v>195</v>
+      </c>
+      <c r="E14" s="17" t="str">
         <f>INT((Table1[[#This Row],[current section]]/Table1[[#This Row],[total sections]])*100)&amp;"%"</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="F14" s="17" t="s">
-        <v>109</v>
+        <v>11%</v>
+      </c>
+      <c r="F14" s="18" t="s">
+        <v>194</v>
       </c>
       <c r="G14" s="18"/>
-      <c r="H14" s="16"/>
-      <c r="I14" s="16"/>
-      <c r="J14" s="16"/>
-      <c r="K14" s="16"/>
-      <c r="L14" s="16" t="s">
-        <v>106</v>
-      </c>
-      <c r="M14" s="16" t="s">
-        <v>107</v>
-      </c>
-      <c r="N14" s="16" t="s">
-        <v>108</v>
+      <c r="H14" s="19">
+        <v>45117</v>
+      </c>
+      <c r="I14" s="17"/>
+      <c r="J14" s="17">
+        <v>3</v>
+      </c>
+      <c r="K14" s="17">
+        <v>26</v>
+      </c>
+      <c r="L14" s="17" t="e">
+        <f>-L21</f>
+        <v>#VALUE!</v>
+      </c>
+      <c r="M14" s="17"/>
+      <c r="N14" s="17" t="s">
+        <v>141</v>
       </c>
       <c r="R14" s="1"/>
       <c r="U14" s="1"/>
     </row>
     <row r="15" spans="1:51" s="5" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="19" t="s">
-        <v>74</v>
-      </c>
-      <c r="B15" s="19" t="s">
-        <v>11</v>
-      </c>
-      <c r="C15" s="19"/>
-      <c r="D15" s="19" t="s">
-        <v>166</v>
-      </c>
-      <c r="E15" s="19" t="e">
+      <c r="A15" s="17">
+        <v>2023</v>
+      </c>
+      <c r="B15" s="17" t="s">
+        <v>11</v>
+      </c>
+      <c r="C15" s="17"/>
+      <c r="D15" s="17" t="s">
+        <v>161</v>
+      </c>
+      <c r="E15" s="17" t="str">
         <f>INT((Table1[[#This Row],[current section]]/Table1[[#This Row],[total sections]])*100)&amp;"%"</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="F15" s="20" t="s">
-        <v>182</v>
-      </c>
-      <c r="G15" s="21"/>
-      <c r="H15" s="19"/>
-      <c r="I15" s="19"/>
-      <c r="J15" s="19"/>
-      <c r="K15" s="19"/>
-      <c r="L15" s="19" t="s">
-        <v>121</v>
-      </c>
-      <c r="M15" s="19" t="s">
-        <v>122</v>
-      </c>
-      <c r="N15" s="19" t="s">
-        <v>112</v>
+        <v>57%</v>
+      </c>
+      <c r="F15" s="18" t="s">
+        <v>173</v>
+      </c>
+      <c r="G15" s="18" t="s">
+        <v>196</v>
+      </c>
+      <c r="H15" s="19" t="s">
+        <v>174</v>
+      </c>
+      <c r="I15" s="17"/>
+      <c r="J15" s="17">
+        <v>11</v>
+      </c>
+      <c r="K15" s="17">
+        <v>19</v>
+      </c>
+      <c r="L15" s="17" t="s">
+        <v>171</v>
+      </c>
+      <c r="M15" s="17" t="s">
+        <v>172</v>
+      </c>
+      <c r="N15" s="17" t="s">
+        <v>141</v>
       </c>
       <c r="P15"/>
       <c r="Q15"/>
@@ -2322,77 +2245,67 @@
       <c r="AY15"/>
     </row>
     <row r="16" spans="1:51" x14ac:dyDescent="0.25">
-      <c r="A16" s="16" t="s">
-        <v>25</v>
-      </c>
-      <c r="B16" s="16" t="s">
-        <v>11</v>
-      </c>
-      <c r="C16" s="16"/>
-      <c r="D16" s="16" t="s">
-        <v>161</v>
-      </c>
-      <c r="E16" s="16" t="e">
+      <c r="A16" s="11" t="s">
+        <v>30</v>
+      </c>
+      <c r="B16" s="11" t="s">
+        <v>11</v>
+      </c>
+      <c r="C16" s="11"/>
+      <c r="D16" s="11" t="s">
+        <v>167</v>
+      </c>
+      <c r="E16" s="11" t="e">
         <f>INT((Table1[[#This Row],[current section]]/Table1[[#This Row],[total sections]])*100)&amp;"%"</f>
         <v>#DIV/0!</v>
       </c>
-      <c r="F16" s="17" t="s">
-        <v>150</v>
-      </c>
-      <c r="G16" s="18"/>
-      <c r="H16" s="16"/>
-      <c r="I16" s="16"/>
-      <c r="J16" s="16"/>
-      <c r="K16" s="16"/>
-      <c r="L16" s="16" t="s">
-        <v>148</v>
-      </c>
-      <c r="M16" s="16" t="s">
-        <v>149</v>
-      </c>
-      <c r="N16" s="16" t="s">
-        <v>131</v>
+      <c r="F16" s="11" t="s">
+        <v>177</v>
+      </c>
+      <c r="G16" s="11"/>
+      <c r="H16" s="11"/>
+      <c r="I16" s="11"/>
+      <c r="J16" s="11"/>
+      <c r="K16" s="11"/>
+      <c r="L16" s="11" t="s">
+        <v>92</v>
+      </c>
+      <c r="M16" s="11" t="s">
+        <v>93</v>
+      </c>
+      <c r="N16" s="11" t="s">
+        <v>94</v>
       </c>
     </row>
     <row r="17" spans="1:51" s="7" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="22">
-        <v>2023</v>
-      </c>
-      <c r="B17" s="22" t="s">
-        <v>11</v>
-      </c>
-      <c r="C17" s="22"/>
-      <c r="D17" s="22" t="s">
-        <v>161</v>
-      </c>
-      <c r="E17" s="22" t="str">
+      <c r="A17" s="13" t="s">
+        <v>30</v>
+      </c>
+      <c r="B17" s="13" t="s">
+        <v>11</v>
+      </c>
+      <c r="C17" s="13"/>
+      <c r="D17" s="13"/>
+      <c r="E17" s="13" t="e">
         <f>INT((Table1[[#This Row],[current section]]/Table1[[#This Row],[total sections]])*100)&amp;"%"</f>
-        <v>57%</v>
-      </c>
-      <c r="F17" s="23" t="s">
-        <v>173</v>
-      </c>
-      <c r="G17" s="24" t="s">
-        <v>196</v>
-      </c>
-      <c r="H17" s="25" t="s">
-        <v>174</v>
-      </c>
-      <c r="I17" s="22"/>
-      <c r="J17" s="22">
-        <v>11</v>
-      </c>
-      <c r="K17" s="22">
-        <v>19</v>
-      </c>
-      <c r="L17" s="22" t="s">
-        <v>171</v>
-      </c>
-      <c r="M17" s="22" t="s">
-        <v>172</v>
-      </c>
-      <c r="N17" s="22" t="s">
-        <v>141</v>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="F17" s="14" t="s">
+        <v>187</v>
+      </c>
+      <c r="G17" s="14"/>
+      <c r="H17" s="13"/>
+      <c r="I17" s="13"/>
+      <c r="J17" s="13"/>
+      <c r="K17" s="13"/>
+      <c r="L17" s="13" t="s">
+        <v>114</v>
+      </c>
+      <c r="M17" s="13" t="s">
+        <v>115</v>
+      </c>
+      <c r="N17" s="13" t="s">
+        <v>116</v>
       </c>
       <c r="P17"/>
       <c r="Q17"/>
@@ -2432,102 +2345,102 @@
       <c r="AY17"/>
     </row>
     <row r="18" spans="1:51" x14ac:dyDescent="0.25">
-      <c r="A18" s="16" t="s">
-        <v>25</v>
-      </c>
-      <c r="B18" s="16" t="s">
-        <v>11</v>
-      </c>
-      <c r="C18" s="16"/>
-      <c r="D18" s="16" t="s">
-        <v>164</v>
-      </c>
-      <c r="E18" s="16" t="e">
+      <c r="A18" s="11" t="s">
+        <v>20</v>
+      </c>
+      <c r="B18" s="11" t="s">
+        <v>11</v>
+      </c>
+      <c r="C18" s="11"/>
+      <c r="D18" s="11" t="s">
+        <v>167</v>
+      </c>
+      <c r="E18" s="11" t="e">
         <f>INT((Table1[[#This Row],[current section]]/Table1[[#This Row],[total sections]])*100)&amp;"%"</f>
         <v>#DIV/0!</v>
       </c>
-      <c r="F18" s="17" t="s">
-        <v>183</v>
-      </c>
-      <c r="G18" s="18"/>
-      <c r="H18" s="16"/>
-      <c r="I18" s="16"/>
-      <c r="J18" s="16"/>
-      <c r="K18" s="16"/>
-      <c r="L18" s="16" t="s">
-        <v>101</v>
-      </c>
-      <c r="M18" s="16" t="s">
-        <v>102</v>
-      </c>
-      <c r="N18" s="16" t="s">
-        <v>103</v>
+      <c r="F18" s="12" t="s">
+        <v>132</v>
+      </c>
+      <c r="G18" s="12"/>
+      <c r="H18" s="11"/>
+      <c r="I18" s="11"/>
+      <c r="J18" s="11"/>
+      <c r="K18" s="11"/>
+      <c r="L18" s="11" t="s">
+        <v>129</v>
+      </c>
+      <c r="M18" s="11" t="s">
+        <v>130</v>
+      </c>
+      <c r="N18" s="11" t="s">
+        <v>131</v>
       </c>
     </row>
     <row r="19" spans="1:51" x14ac:dyDescent="0.25">
-      <c r="A19" s="16" t="s">
+      <c r="A19" s="11" t="s">
         <v>74</v>
       </c>
-      <c r="B19" s="16" t="s">
-        <v>11</v>
-      </c>
-      <c r="C19" s="16"/>
-      <c r="D19" s="16" t="s">
-        <v>164</v>
-      </c>
-      <c r="E19" s="16" t="e">
+      <c r="B19" s="11" t="s">
+        <v>11</v>
+      </c>
+      <c r="C19" s="11"/>
+      <c r="D19" s="11" t="s">
+        <v>167</v>
+      </c>
+      <c r="E19" s="11" t="e">
         <f>INT((Table1[[#This Row],[current section]]/Table1[[#This Row],[total sections]])*100)&amp;"%"</f>
         <v>#DIV/0!</v>
       </c>
-      <c r="F19" s="17" t="s">
-        <v>185</v>
-      </c>
-      <c r="G19" s="18"/>
-      <c r="H19" s="16"/>
-      <c r="I19" s="16"/>
-      <c r="J19" s="16"/>
-      <c r="K19" s="16"/>
-      <c r="L19" s="16" t="s">
-        <v>123</v>
-      </c>
-      <c r="M19" s="16" t="s">
-        <v>124</v>
-      </c>
-      <c r="N19" s="16" t="s">
-        <v>125</v>
+      <c r="F19" s="12" t="s">
+        <v>202</v>
+      </c>
+      <c r="G19" s="12"/>
+      <c r="H19" s="11"/>
+      <c r="I19" s="11"/>
+      <c r="J19" s="11"/>
+      <c r="K19" s="11"/>
+      <c r="L19" s="11" t="s">
+        <v>143</v>
+      </c>
+      <c r="M19" s="11" t="s">
+        <v>144</v>
+      </c>
+      <c r="N19" s="11" t="s">
+        <v>50</v>
       </c>
     </row>
     <row r="20" spans="1:51" s="3" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A20" s="12">
-        <v>2020</v>
-      </c>
-      <c r="B20" s="12" t="s">
-        <v>11</v>
-      </c>
-      <c r="C20" s="12"/>
-      <c r="D20" s="12" t="s">
-        <v>164</v>
-      </c>
-      <c r="E20" s="12" t="e">
+      <c r="A20" s="15" t="s">
+        <v>74</v>
+      </c>
+      <c r="B20" s="15" t="s">
+        <v>11</v>
+      </c>
+      <c r="C20" s="15"/>
+      <c r="D20" s="15" t="s">
+        <v>166</v>
+      </c>
+      <c r="E20" s="15" t="e">
         <f>INT((Table1[[#This Row],[current section]]/Table1[[#This Row],[total sections]])*100)&amp;"%"</f>
         <v>#DIV/0!</v>
       </c>
-      <c r="F20" s="13" t="s">
-        <v>184</v>
-      </c>
-      <c r="G20" s="14"/>
-      <c r="H20" s="12"/>
-      <c r="I20" s="12"/>
-      <c r="J20" s="12"/>
-      <c r="K20" s="12"/>
-      <c r="L20" s="12" t="s">
-        <v>104</v>
-      </c>
-      <c r="M20" s="12" t="s">
-        <v>105</v>
-      </c>
-      <c r="N20" s="12" t="s">
-        <v>103</v>
+      <c r="F20" s="16" t="s">
+        <v>182</v>
+      </c>
+      <c r="G20" s="16"/>
+      <c r="H20" s="15"/>
+      <c r="I20" s="15"/>
+      <c r="J20" s="15"/>
+      <c r="K20" s="15"/>
+      <c r="L20" s="15" t="s">
+        <v>121</v>
+      </c>
+      <c r="M20" s="15" t="s">
+        <v>122</v>
+      </c>
+      <c r="N20" s="15" t="s">
+        <v>112</v>
       </c>
       <c r="P20"/>
       <c r="Q20"/>
@@ -2567,129 +2480,133 @@
       <c r="AY20"/>
     </row>
     <row r="21" spans="1:51" x14ac:dyDescent="0.25">
-      <c r="A21" s="16" t="s">
-        <v>35</v>
-      </c>
-      <c r="B21" s="16" t="s">
-        <v>11</v>
-      </c>
-      <c r="C21" s="16"/>
-      <c r="D21" s="16" t="s">
-        <v>170</v>
-      </c>
-      <c r="E21" s="16" t="e">
+      <c r="A21" s="13" t="s">
+        <v>74</v>
+      </c>
+      <c r="B21" s="13" t="s">
+        <v>11</v>
+      </c>
+      <c r="C21" s="13"/>
+      <c r="D21" s="13" t="s">
+        <v>164</v>
+      </c>
+      <c r="E21" s="13" t="e">
         <f>INT((Table1[[#This Row],[current section]]/Table1[[#This Row],[total sections]])*100)&amp;"%"</f>
         <v>#DIV/0!</v>
       </c>
-      <c r="F21" s="17" t="s">
-        <v>186</v>
-      </c>
-      <c r="G21" s="18"/>
-      <c r="H21" s="16"/>
-      <c r="I21" s="16"/>
-      <c r="J21" s="16"/>
-      <c r="K21" s="16"/>
-      <c r="L21" s="16" t="s">
-        <v>95</v>
-      </c>
-      <c r="M21" s="16" t="s">
-        <v>96</v>
-      </c>
-      <c r="N21" s="16" t="s">
-        <v>97</v>
+      <c r="F21" s="14" t="s">
+        <v>185</v>
+      </c>
+      <c r="G21" s="14"/>
+      <c r="H21" s="13"/>
+      <c r="I21" s="13"/>
+      <c r="J21" s="13"/>
+      <c r="K21" s="13"/>
+      <c r="L21" s="13" t="s">
+        <v>123</v>
+      </c>
+      <c r="M21" s="13" t="s">
+        <v>124</v>
+      </c>
+      <c r="N21" s="13" t="s">
+        <v>125</v>
       </c>
     </row>
     <row r="22" spans="1:51" x14ac:dyDescent="0.25">
-      <c r="A22" s="16" t="s">
-        <v>25</v>
-      </c>
-      <c r="B22" s="16" t="s">
-        <v>11</v>
-      </c>
-      <c r="C22" s="16"/>
-      <c r="D22" s="16"/>
-      <c r="E22" s="16" t="e">
+      <c r="A22" s="13" t="s">
+        <v>74</v>
+      </c>
+      <c r="B22" s="13" t="s">
+        <v>11</v>
+      </c>
+      <c r="C22" s="13"/>
+      <c r="D22" s="13"/>
+      <c r="E22" s="13" t="e">
         <f>INT((Table1[[#This Row],[current section]]/Table1[[#This Row],[total sections]])*100)&amp;"%"</f>
         <v>#DIV/0!</v>
       </c>
-      <c r="F22" s="17" t="s">
-        <v>142</v>
-      </c>
-      <c r="G22" s="18"/>
-      <c r="H22" s="16"/>
-      <c r="I22" s="16"/>
-      <c r="J22" s="16"/>
-      <c r="K22" s="16"/>
-      <c r="L22" s="16" t="s">
-        <v>139</v>
-      </c>
-      <c r="M22" s="16" t="s">
-        <v>140</v>
-      </c>
-      <c r="N22" s="16" t="s">
-        <v>141</v>
+      <c r="F22" s="14" t="s">
+        <v>113</v>
+      </c>
+      <c r="G22" s="14"/>
+      <c r="H22" s="13"/>
+      <c r="I22" s="13"/>
+      <c r="J22" s="13"/>
+      <c r="K22" s="13"/>
+      <c r="L22" s="13" t="s">
+        <v>110</v>
+      </c>
+      <c r="M22" s="13" t="s">
+        <v>111</v>
+      </c>
+      <c r="N22" s="13" t="s">
+        <v>112</v>
       </c>
     </row>
     <row r="23" spans="1:51" x14ac:dyDescent="0.25">
-      <c r="A23" s="16" t="s">
-        <v>25</v>
-      </c>
-      <c r="B23" s="16" t="s">
-        <v>11</v>
-      </c>
-      <c r="C23" s="16"/>
-      <c r="D23" s="16"/>
-      <c r="E23" s="16" t="e">
+      <c r="A23" s="13" t="s">
+        <v>35</v>
+      </c>
+      <c r="B23" s="13" t="s">
+        <v>11</v>
+      </c>
+      <c r="C23" s="13"/>
+      <c r="D23" s="13" t="s">
+        <v>169</v>
+      </c>
+      <c r="E23" s="13" t="e">
         <f>INT((Table1[[#This Row],[current section]]/Table1[[#This Row],[total sections]])*100)&amp;"%"</f>
         <v>#DIV/0!</v>
       </c>
-      <c r="F23" s="17" t="s">
-        <v>147</v>
-      </c>
-      <c r="G23" s="18"/>
-      <c r="H23" s="16"/>
-      <c r="I23" s="16"/>
-      <c r="J23" s="16"/>
-      <c r="K23" s="16"/>
-      <c r="L23" s="16" t="s">
-        <v>145</v>
-      </c>
-      <c r="M23" s="16" t="s">
-        <v>146</v>
-      </c>
-      <c r="N23" s="16" t="s">
-        <v>108</v>
+      <c r="F23" s="14" t="s">
+        <v>189</v>
+      </c>
+      <c r="G23" s="14"/>
+      <c r="H23" s="13"/>
+      <c r="I23" s="13"/>
+      <c r="J23" s="13"/>
+      <c r="K23" s="13"/>
+      <c r="L23" s="13" t="s">
+        <v>98</v>
+      </c>
+      <c r="M23" s="13" t="s">
+        <v>99</v>
+      </c>
+      <c r="N23" s="13" t="s">
+        <v>100</v>
       </c>
     </row>
     <row r="24" spans="1:51" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A24" s="16" t="s">
-        <v>74</v>
-      </c>
-      <c r="B24" s="16" t="s">
-        <v>11</v>
-      </c>
-      <c r="C24" s="16"/>
-      <c r="D24" s="16"/>
-      <c r="E24" s="16" t="e">
+      <c r="A24" s="13" t="s">
+        <v>35</v>
+      </c>
+      <c r="B24" s="13" t="s">
+        <v>11</v>
+      </c>
+      <c r="C24" s="13"/>
+      <c r="D24" s="13" t="s">
+        <v>163</v>
+      </c>
+      <c r="E24" s="13" t="e">
         <f>INT((Table1[[#This Row],[current section]]/Table1[[#This Row],[total sections]])*100)&amp;"%"</f>
         <v>#DIV/0!</v>
       </c>
-      <c r="F24" s="17" t="s">
-        <v>113</v>
-      </c>
-      <c r="G24" s="18"/>
-      <c r="H24" s="16"/>
-      <c r="I24" s="16"/>
-      <c r="J24" s="16"/>
-      <c r="K24" s="16"/>
-      <c r="L24" s="16" t="s">
-        <v>110</v>
-      </c>
-      <c r="M24" s="16" t="s">
-        <v>111</v>
-      </c>
-      <c r="N24" s="16" t="s">
-        <v>112</v>
+      <c r="F24" s="14" t="s">
+        <v>120</v>
+      </c>
+      <c r="G24" s="14"/>
+      <c r="H24" s="13"/>
+      <c r="I24" s="13"/>
+      <c r="J24" s="13"/>
+      <c r="K24" s="13"/>
+      <c r="L24" s="13" t="s">
+        <v>117</v>
+      </c>
+      <c r="M24" s="13" t="s">
+        <v>118</v>
+      </c>
+      <c r="N24" s="13" t="s">
+        <v>119</v>
       </c>
       <c r="P24"/>
       <c r="Q24"/>
@@ -2729,34 +2646,36 @@
       <c r="AY24"/>
     </row>
     <row r="25" spans="1:51" s="4" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A25" s="16" t="s">
-        <v>30</v>
-      </c>
-      <c r="B25" s="16" t="s">
-        <v>11</v>
-      </c>
-      <c r="C25" s="16"/>
-      <c r="D25" s="16"/>
-      <c r="E25" s="16" t="e">
+      <c r="A25" s="13" t="s">
+        <v>35</v>
+      </c>
+      <c r="B25" s="13" t="s">
+        <v>11</v>
+      </c>
+      <c r="C25" s="13"/>
+      <c r="D25" s="13" t="s">
+        <v>163</v>
+      </c>
+      <c r="E25" s="13" t="e">
         <f>INT((Table1[[#This Row],[current section]]/Table1[[#This Row],[total sections]])*100)&amp;"%"</f>
         <v>#DIV/0!</v>
       </c>
-      <c r="F25" s="17" t="s">
-        <v>187</v>
-      </c>
-      <c r="G25" s="18"/>
-      <c r="H25" s="16"/>
-      <c r="I25" s="16"/>
-      <c r="J25" s="16"/>
-      <c r="K25" s="16"/>
-      <c r="L25" s="16" t="s">
-        <v>114</v>
-      </c>
-      <c r="M25" s="16" t="s">
-        <v>115</v>
-      </c>
-      <c r="N25" s="16" t="s">
-        <v>116</v>
+      <c r="F25" s="14" t="s">
+        <v>179</v>
+      </c>
+      <c r="G25" s="14"/>
+      <c r="H25" s="13"/>
+      <c r="I25" s="13"/>
+      <c r="J25" s="13"/>
+      <c r="K25" s="13"/>
+      <c r="L25" s="13" t="s">
+        <v>137</v>
+      </c>
+      <c r="M25" s="13" t="s">
+        <v>138</v>
+      </c>
+      <c r="N25" s="13" t="s">
+        <v>100</v>
       </c>
       <c r="P25"/>
       <c r="Q25"/>
@@ -2796,258 +2715,341 @@
       <c r="AY25"/>
     </row>
     <row r="26" spans="1:51" x14ac:dyDescent="0.25">
-      <c r="A26" s="16"/>
-      <c r="B26" s="16" t="s">
-        <v>215</v>
-      </c>
-      <c r="C26" s="16"/>
-      <c r="D26" s="16" t="s">
-        <v>200</v>
-      </c>
-      <c r="E26" s="16" t="e">
+      <c r="A26" s="13" t="s">
+        <v>35</v>
+      </c>
+      <c r="B26" s="13" t="s">
+        <v>11</v>
+      </c>
+      <c r="C26" s="13"/>
+      <c r="D26" s="13" t="s">
+        <v>170</v>
+      </c>
+      <c r="E26" s="13" t="e">
         <f>INT((Table1[[#This Row],[current section]]/Table1[[#This Row],[total sections]])*100)&amp;"%"</f>
         <v>#DIV/0!</v>
       </c>
-      <c r="F26" s="17" t="s">
-        <v>214</v>
-      </c>
-      <c r="G26" s="18"/>
-      <c r="H26" s="16"/>
-      <c r="I26" s="16"/>
-      <c r="J26" s="16"/>
-      <c r="K26" s="16"/>
-      <c r="L26" s="16"/>
-      <c r="M26" s="16"/>
-      <c r="N26" s="16"/>
+      <c r="F26" s="14" t="s">
+        <v>186</v>
+      </c>
+      <c r="G26" s="14"/>
+      <c r="H26" s="13"/>
+      <c r="I26" s="13"/>
+      <c r="J26" s="13"/>
+      <c r="K26" s="13"/>
+      <c r="L26" s="13" t="s">
+        <v>95</v>
+      </c>
+      <c r="M26" s="13" t="s">
+        <v>96</v>
+      </c>
+      <c r="N26" s="13" t="s">
+        <v>97</v>
+      </c>
     </row>
     <row r="27" spans="1:51" x14ac:dyDescent="0.25">
-      <c r="A27" s="16"/>
-      <c r="B27" s="16" t="s">
-        <v>215</v>
-      </c>
-      <c r="C27" s="16"/>
-      <c r="D27" s="16" t="s">
-        <v>217</v>
-      </c>
-      <c r="E27" s="26">
-        <v>0.15</v>
-      </c>
-      <c r="F27" s="17" t="s">
-        <v>206</v>
-      </c>
-      <c r="G27" s="18"/>
-      <c r="H27" s="16"/>
-      <c r="I27" s="16"/>
-      <c r="J27" s="16"/>
-      <c r="K27" s="16"/>
-      <c r="L27" s="16"/>
-      <c r="M27" s="16"/>
-      <c r="N27" s="16"/>
-    </row>
-    <row r="28" spans="1:51" x14ac:dyDescent="0.25">
-      <c r="A28" s="16"/>
-      <c r="B28" s="16" t="s">
-        <v>215</v>
-      </c>
-      <c r="C28" s="16"/>
-      <c r="D28" s="16" t="s">
-        <v>218</v>
-      </c>
-      <c r="E28" s="26">
-        <v>0.7</v>
-      </c>
-      <c r="F28" s="17" t="s">
-        <v>207</v>
-      </c>
-      <c r="G28" s="18"/>
-      <c r="H28" s="16"/>
-      <c r="I28" s="16"/>
-      <c r="J28" s="16"/>
-      <c r="K28" s="16"/>
-      <c r="L28" s="16"/>
-      <c r="M28" s="16"/>
-      <c r="N28" s="16"/>
-    </row>
-    <row r="29" spans="1:51" x14ac:dyDescent="0.25">
-      <c r="A29" s="16"/>
-      <c r="B29" s="16" t="s">
-        <v>215</v>
-      </c>
-      <c r="C29" s="16"/>
-      <c r="D29" s="16" t="s">
-        <v>219</v>
-      </c>
-      <c r="E29" s="26">
-        <v>0.46</v>
-      </c>
-      <c r="F29" s="17" t="s">
-        <v>208</v>
-      </c>
-      <c r="G29" s="18"/>
-      <c r="H29" s="16"/>
-      <c r="I29" s="16"/>
-      <c r="J29" s="16"/>
-      <c r="K29" s="16"/>
-      <c r="L29" s="16"/>
-      <c r="M29" s="16"/>
-      <c r="N29" s="16"/>
-    </row>
-    <row r="30" spans="1:51" x14ac:dyDescent="0.25">
-      <c r="A30" s="16"/>
-      <c r="B30" s="16" t="s">
-        <v>215</v>
-      </c>
-      <c r="C30" s="16"/>
-      <c r="D30" s="16" t="s">
-        <v>220</v>
-      </c>
-      <c r="E30" s="26">
-        <v>0.78</v>
-      </c>
-      <c r="F30" s="17" t="s">
-        <v>209</v>
-      </c>
-      <c r="G30" s="18"/>
-      <c r="H30" s="16"/>
-      <c r="I30" s="16"/>
-      <c r="J30" s="16"/>
-      <c r="K30" s="16"/>
-      <c r="L30" s="16"/>
-      <c r="M30" s="16"/>
-      <c r="N30" s="16"/>
-    </row>
-    <row r="31" spans="1:51" x14ac:dyDescent="0.25">
-      <c r="A31" s="16"/>
-      <c r="B31" s="16" t="s">
-        <v>215</v>
-      </c>
-      <c r="C31" s="16"/>
-      <c r="D31" s="16" t="s">
-        <v>221</v>
-      </c>
-      <c r="E31" s="16" t="e">
+      <c r="A27" s="15" t="s">
+        <v>25</v>
+      </c>
+      <c r="B27" s="15" t="s">
+        <v>11</v>
+      </c>
+      <c r="C27" s="15"/>
+      <c r="D27" s="15" t="s">
+        <v>160</v>
+      </c>
+      <c r="E27" s="15" t="e">
         <f>INT((Table1[[#This Row],[current section]]/Table1[[#This Row],[total sections]])*100)&amp;"%"</f>
         <v>#DIV/0!</v>
       </c>
-      <c r="F31" s="17" t="s">
-        <v>212</v>
-      </c>
-      <c r="G31" s="18"/>
-      <c r="H31" s="16"/>
-      <c r="I31" s="16"/>
-      <c r="J31" s="16"/>
-      <c r="K31" s="16"/>
-      <c r="L31" s="16"/>
-      <c r="M31" s="16"/>
-      <c r="N31" s="16"/>
-    </row>
-    <row r="32" spans="1:51" x14ac:dyDescent="0.25">
-      <c r="A32" s="16"/>
-      <c r="B32" s="16" t="s">
-        <v>215</v>
-      </c>
-      <c r="C32" s="16"/>
-      <c r="D32" s="16" t="s">
-        <v>166</v>
-      </c>
-      <c r="E32" s="26">
-        <v>0.15</v>
-      </c>
-      <c r="F32" s="17" t="s">
-        <v>210</v>
-      </c>
-      <c r="G32" s="18"/>
-      <c r="H32" s="16"/>
-      <c r="I32" s="16"/>
-      <c r="J32" s="16"/>
-      <c r="K32" s="16"/>
-      <c r="L32" s="16"/>
-      <c r="M32" s="16"/>
-      <c r="N32" s="16"/>
-    </row>
-    <row r="33" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A33" s="16"/>
-      <c r="B33" s="16" t="s">
-        <v>215</v>
-      </c>
-      <c r="C33" s="16"/>
-      <c r="D33" s="16" t="s">
-        <v>222</v>
-      </c>
-      <c r="E33" s="16" t="e">
+      <c r="F27" s="16" t="s">
+        <v>188</v>
+      </c>
+      <c r="G27" s="16"/>
+      <c r="H27" s="15"/>
+      <c r="I27" s="15"/>
+      <c r="J27" s="15"/>
+      <c r="K27" s="15"/>
+      <c r="L27" s="15" t="s">
+        <v>126</v>
+      </c>
+      <c r="M27" s="15" t="s">
+        <v>127</v>
+      </c>
+      <c r="N27" s="15" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="28" spans="1:51" x14ac:dyDescent="0.25">
+      <c r="A28" s="13" t="s">
+        <v>25</v>
+      </c>
+      <c r="B28" s="13" t="s">
+        <v>11</v>
+      </c>
+      <c r="C28" s="13"/>
+      <c r="D28" s="13" t="s">
+        <v>163</v>
+      </c>
+      <c r="E28" s="13" t="e">
         <f>INT((Table1[[#This Row],[current section]]/Table1[[#This Row],[total sections]])*100)&amp;"%"</f>
         <v>#DIV/0!</v>
       </c>
-      <c r="F33" s="17" t="s">
-        <v>211</v>
-      </c>
-      <c r="G33" s="18"/>
-      <c r="H33" s="16"/>
-      <c r="I33" s="16"/>
-      <c r="J33" s="16"/>
-      <c r="K33" s="16"/>
-      <c r="L33" s="16"/>
-      <c r="M33" s="16"/>
-      <c r="N33" s="16"/>
+      <c r="F28" s="14" t="s">
+        <v>180</v>
+      </c>
+      <c r="G28" s="14"/>
+      <c r="H28" s="13"/>
+      <c r="I28" s="13"/>
+      <c r="J28" s="13"/>
+      <c r="K28" s="13"/>
+      <c r="L28" s="13" t="s">
+        <v>135</v>
+      </c>
+      <c r="M28" s="13" t="s">
+        <v>136</v>
+      </c>
+      <c r="N28" s="13" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="29" spans="1:51" x14ac:dyDescent="0.25">
+      <c r="A29" s="13" t="s">
+        <v>25</v>
+      </c>
+      <c r="B29" s="13" t="s">
+        <v>11</v>
+      </c>
+      <c r="C29" s="13"/>
+      <c r="D29" s="13" t="s">
+        <v>168</v>
+      </c>
+      <c r="E29" s="13" t="e">
+        <f>INT((Table1[[#This Row],[current section]]/Table1[[#This Row],[total sections]])*100)&amp;"%"</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="F29" s="14" t="s">
+        <v>181</v>
+      </c>
+      <c r="G29" s="14"/>
+      <c r="H29" s="13"/>
+      <c r="I29" s="13"/>
+      <c r="J29" s="13"/>
+      <c r="K29" s="13"/>
+      <c r="L29" s="13" t="s">
+        <v>133</v>
+      </c>
+      <c r="M29" s="13" t="s">
+        <v>134</v>
+      </c>
+      <c r="N29" s="13" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="30" spans="1:51" x14ac:dyDescent="0.25">
+      <c r="A30" s="13" t="s">
+        <v>25</v>
+      </c>
+      <c r="B30" s="13" t="s">
+        <v>11</v>
+      </c>
+      <c r="C30" s="13"/>
+      <c r="D30" s="13" t="s">
+        <v>162</v>
+      </c>
+      <c r="E30" s="13" t="e">
+        <f>INT((Table1[[#This Row],[current section]]/Table1[[#This Row],[total sections]])*100)&amp;"%"</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="F30" s="14" t="s">
+        <v>109</v>
+      </c>
+      <c r="G30" s="14"/>
+      <c r="H30" s="13"/>
+      <c r="I30" s="13"/>
+      <c r="J30" s="13"/>
+      <c r="K30" s="13"/>
+      <c r="L30" s="13" t="s">
+        <v>106</v>
+      </c>
+      <c r="M30" s="13" t="s">
+        <v>107</v>
+      </c>
+      <c r="N30" s="13" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="31" spans="1:51" x14ac:dyDescent="0.25">
+      <c r="A31" s="13" t="s">
+        <v>25</v>
+      </c>
+      <c r="B31" s="13" t="s">
+        <v>11</v>
+      </c>
+      <c r="C31" s="13"/>
+      <c r="D31" s="13" t="s">
+        <v>161</v>
+      </c>
+      <c r="E31" s="13" t="e">
+        <f>INT((Table1[[#This Row],[current section]]/Table1[[#This Row],[total sections]])*100)&amp;"%"</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="F31" s="14" t="s">
+        <v>150</v>
+      </c>
+      <c r="G31" s="14"/>
+      <c r="H31" s="13"/>
+      <c r="I31" s="13"/>
+      <c r="J31" s="13"/>
+      <c r="K31" s="13"/>
+      <c r="L31" s="13" t="s">
+        <v>148</v>
+      </c>
+      <c r="M31" s="13" t="s">
+        <v>149</v>
+      </c>
+      <c r="N31" s="13" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="32" spans="1:51" x14ac:dyDescent="0.25">
+      <c r="A32" s="13" t="s">
+        <v>25</v>
+      </c>
+      <c r="B32" s="13" t="s">
+        <v>11</v>
+      </c>
+      <c r="C32" s="13"/>
+      <c r="D32" s="13" t="s">
+        <v>164</v>
+      </c>
+      <c r="E32" s="13" t="e">
+        <f>INT((Table1[[#This Row],[current section]]/Table1[[#This Row],[total sections]])*100)&amp;"%"</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="F32" s="14" t="s">
+        <v>183</v>
+      </c>
+      <c r="G32" s="14"/>
+      <c r="H32" s="13"/>
+      <c r="I32" s="13"/>
+      <c r="J32" s="13"/>
+      <c r="K32" s="13"/>
+      <c r="L32" s="13" t="s">
+        <v>101</v>
+      </c>
+      <c r="M32" s="13" t="s">
+        <v>102</v>
+      </c>
+      <c r="N32" s="13" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="33" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A33" s="13" t="s">
+        <v>25</v>
+      </c>
+      <c r="B33" s="13" t="s">
+        <v>11</v>
+      </c>
+      <c r="C33" s="13"/>
+      <c r="D33" s="13"/>
+      <c r="E33" s="13" t="e">
+        <f>INT((Table1[[#This Row],[current section]]/Table1[[#This Row],[total sections]])*100)&amp;"%"</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="F33" s="14" t="s">
+        <v>142</v>
+      </c>
+      <c r="G33" s="14"/>
+      <c r="H33" s="13"/>
+      <c r="I33" s="13"/>
+      <c r="J33" s="13"/>
+      <c r="K33" s="13"/>
+      <c r="L33" s="13" t="s">
+        <v>139</v>
+      </c>
+      <c r="M33" s="13" t="s">
+        <v>140</v>
+      </c>
+      <c r="N33" s="13" t="s">
+        <v>141</v>
+      </c>
     </row>
     <row r="34" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A34" s="16"/>
-      <c r="B34" s="16" t="s">
-        <v>215</v>
-      </c>
-      <c r="C34" s="16"/>
-      <c r="D34" s="16" t="s">
-        <v>223</v>
-      </c>
-      <c r="E34" s="26">
-        <v>0.86</v>
-      </c>
-      <c r="F34" s="17" t="s">
-        <v>213</v>
-      </c>
-      <c r="G34" s="18"/>
-      <c r="H34" s="16"/>
-      <c r="I34" s="16"/>
-      <c r="J34" s="16"/>
-      <c r="K34" s="16"/>
-      <c r="L34" s="16"/>
-      <c r="M34" s="16"/>
-      <c r="N34" s="16"/>
+      <c r="A34" s="13" t="s">
+        <v>25</v>
+      </c>
+      <c r="B34" s="13" t="s">
+        <v>11</v>
+      </c>
+      <c r="C34" s="13"/>
+      <c r="D34" s="13"/>
+      <c r="E34" s="13" t="e">
+        <f>INT((Table1[[#This Row],[current section]]/Table1[[#This Row],[total sections]])*100)&amp;"%"</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="F34" s="14" t="s">
+        <v>147</v>
+      </c>
+      <c r="G34" s="14"/>
+      <c r="H34" s="13"/>
+      <c r="I34" s="13"/>
+      <c r="J34" s="13"/>
+      <c r="K34" s="13"/>
+      <c r="L34" s="13" t="s">
+        <v>145</v>
+      </c>
+      <c r="M34" s="13" t="s">
+        <v>146</v>
+      </c>
+      <c r="N34" s="13" t="s">
+        <v>108</v>
+      </c>
     </row>
     <row r="35" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A35" s="16"/>
-      <c r="B35" s="16" t="s">
-        <v>215</v>
-      </c>
-      <c r="C35" s="16"/>
-      <c r="D35" s="16" t="s">
-        <v>160</v>
-      </c>
-      <c r="E35" s="26">
-        <v>0.25</v>
-      </c>
-      <c r="F35" s="17" t="s">
-        <v>216</v>
-      </c>
-      <c r="G35" s="18"/>
-      <c r="H35" s="16"/>
-      <c r="I35" s="16"/>
-      <c r="J35" s="16"/>
-      <c r="K35" s="16"/>
-      <c r="L35" s="16"/>
-      <c r="M35" s="16"/>
-      <c r="N35" s="16"/>
+      <c r="A35" s="13" t="s">
+        <v>10</v>
+      </c>
+      <c r="B35" s="13" t="s">
+        <v>11</v>
+      </c>
+      <c r="C35" s="13"/>
+      <c r="D35" s="13" t="s">
+        <v>165</v>
+      </c>
+      <c r="E35" s="13" t="e">
+        <f>INT((Table1[[#This Row],[current section]]/Table1[[#This Row],[total sections]])*100)&amp;"%"</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="F35" s="14" t="s">
+        <v>178</v>
+      </c>
+      <c r="G35" s="14"/>
+      <c r="H35" s="13"/>
+      <c r="I35" s="13"/>
+      <c r="J35" s="13"/>
+      <c r="K35" s="13"/>
+      <c r="L35" s="13" t="s">
+        <v>151</v>
+      </c>
+      <c r="M35" s="13" t="s">
+        <v>152</v>
+      </c>
+      <c r="N35" s="13" t="s">
+        <v>153</v>
+      </c>
     </row>
     <row r="37" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="E37" s="11" t="str">
+      <c r="E37" s="10" t="str">
         <f>PROPER(F2)</f>
-        <v>Architecting Reactive Angular Applications With Redux A…</v>
+        <v>- Java Programming Masterclass Updated To Java 17</v>
       </c>
     </row>
     <row r="42" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="E42" s="10" t="str">
+      <c r="E42" s="1" t="str">
         <f>PROPER(F16)</f>
-        <v>React - The Complete Guide (Includes Hooks, React Route...</v>
+        <v xml:space="preserve">Learn Angular 2 Development By Building 12 Apps </v>
       </c>
     </row>
   </sheetData>

</xml_diff>